<commit_message>
I added all negative controls, mock communities and probiotics treatments (pos controls) to the NCBI file
</commit_message>
<xml_diff>
--- a/source_data/pigs_samples_IDs_for_NCBI.xlsx
+++ b/source_data/pigs_samples_IDs_for_NCBI.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="28705"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="7920" yWindow="1140" windowWidth="25360" windowHeight="15760"/>
+    <workbookView xWindow="10460" yWindow="0" windowWidth="8000" windowHeight="15760"/>
   </bookViews>
   <sheets>
     <sheet name="MIMARKS.survey.host-associated." sheetId="1" r:id="rId1"/>
@@ -355,7 +355,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14300" uniqueCount="1237">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14345" uniqueCount="1281">
   <si>
     <r>
       <rPr>
@@ -4357,6 +4357,138 @@
   </si>
   <si>
     <t>Fe1/14192</t>
+  </si>
+  <si>
+    <t>Au14/MC1</t>
+  </si>
+  <si>
+    <t>Au14/MC2</t>
+  </si>
+  <si>
+    <t>Au14/MC3</t>
+  </si>
+  <si>
+    <t>Au14/MC4</t>
+  </si>
+  <si>
+    <t>Au14/MC5</t>
+  </si>
+  <si>
+    <t>Au14/MC6</t>
+  </si>
+  <si>
+    <t>Au14/MC7</t>
+  </si>
+  <si>
+    <t>Au14/MC8</t>
+  </si>
+  <si>
+    <t>Au14/MC9</t>
+  </si>
+  <si>
+    <t>18Ja24/ColiGuard_P3</t>
+  </si>
+  <si>
+    <t>18Ja24/Protexin_P4</t>
+  </si>
+  <si>
+    <t>18Ja24/ColiGuard_P4</t>
+  </si>
+  <si>
+    <t>18Ja24/ColiGuard_P5</t>
+  </si>
+  <si>
+    <t>18Ja24/ColiGuard_P6</t>
+  </si>
+  <si>
+    <t>18Ja24/Protexin_P6</t>
+  </si>
+  <si>
+    <t>18Ja24/Protexin_P7</t>
+  </si>
+  <si>
+    <t>18Ja24/ColiGuard_P7</t>
+  </si>
+  <si>
+    <t>18Ja24/Protexin_P8</t>
+  </si>
+  <si>
+    <t>18Ja24/ColiGuard_P8</t>
+  </si>
+  <si>
+    <t>18Ja24/Protexin_P9</t>
+  </si>
+  <si>
+    <t>18Ja24/ColiGuard_P9</t>
+  </si>
+  <si>
+    <t>18Ja24/Protexin_P10</t>
+  </si>
+  <si>
+    <t>18Ja24/ColiGuard_P10</t>
+  </si>
+  <si>
+    <t>18Ja24/Protexin_P3</t>
+  </si>
+  <si>
+    <t>18Ja24/Protexin_P5</t>
+  </si>
+  <si>
+    <t>NA/neg.control_P1</t>
+  </si>
+  <si>
+    <t>NA/neg.control_P1.2</t>
+  </si>
+  <si>
+    <t>NA/neg.control_P2</t>
+  </si>
+  <si>
+    <t>NA/neg.control_P2.2</t>
+  </si>
+  <si>
+    <t>NA/neg.control_P3</t>
+  </si>
+  <si>
+    <t>NA/neg.control_P3.2</t>
+  </si>
+  <si>
+    <t>NA/neg.control_P4</t>
+  </si>
+  <si>
+    <t>NA/neg.control_P4.2</t>
+  </si>
+  <si>
+    <t>NA/neg.control_P5</t>
+  </si>
+  <si>
+    <t>NA/neg.control_P5.2</t>
+  </si>
+  <si>
+    <t>NA/neg.control_P6</t>
+  </si>
+  <si>
+    <t>NA/neg.control_P7</t>
+  </si>
+  <si>
+    <t>NA/neg.control_P7.2</t>
+  </si>
+  <si>
+    <t>NA/neg.control_P8</t>
+  </si>
+  <si>
+    <t>NA/neg.control_P8.2</t>
+  </si>
+  <si>
+    <t>NA/neg.control_P9</t>
+  </si>
+  <si>
+    <t>NA/neg.control_P9.2</t>
+  </si>
+  <si>
+    <t>NA/neg.control_P10</t>
+  </si>
+  <si>
+    <t>NA/neg.control_P10.2</t>
   </si>
 </sst>
 </file>
@@ -4539,8 +4671,40 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="103">
+  <cellStyleXfs count="135">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -4686,7 +4850,7 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="103">
+  <cellStyles count="135">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -4738,6 +4902,22 @@
     <cellStyle name="Followed Hyperlink" xfId="98" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="100" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="102" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="104" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="106" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="108" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="110" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="112" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="114" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="116" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="118" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="120" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="122" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="124" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="126" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="128" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="130" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="132" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="134" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -4789,6 +4969,22 @@
     <cellStyle name="Hyperlink" xfId="97" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="99" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="101" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="103" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="105" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="107" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="109" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="111" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="113" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="115" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="117" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="119" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="121" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="123" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="125" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="127" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="129" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="131" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="133" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -5094,15 +5290,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AA850"/>
+  <dimension ref="A1:AA895"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A120" workbookViewId="0">
-      <selection activeCell="A145" sqref="A145"/>
+    <sheetView tabSelected="1" topLeftCell="A835" workbookViewId="0">
+      <selection activeCell="B875" sqref="B875"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="14.6640625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="19.5" style="1" customWidth="1"/>
     <col min="2" max="2" width="20.5" style="1" customWidth="1"/>
     <col min="3" max="3" width="22.6640625" style="1" customWidth="1"/>
     <col min="4" max="4" width="18.5" style="1" customWidth="1"/>
@@ -51771,6 +51967,231 @@
       </c>
       <c r="R850" s="1" t="s">
         <v>1222</v>
+      </c>
+    </row>
+    <row r="851" spans="1:18">
+      <c r="A851" s="1" t="s">
+        <v>1237</v>
+      </c>
+    </row>
+    <row r="852" spans="1:18">
+      <c r="A852" s="1" t="s">
+        <v>1238</v>
+      </c>
+    </row>
+    <row r="853" spans="1:18">
+      <c r="A853" s="1" t="s">
+        <v>1239</v>
+      </c>
+    </row>
+    <row r="854" spans="1:18">
+      <c r="A854" s="1" t="s">
+        <v>1240</v>
+      </c>
+    </row>
+    <row r="855" spans="1:18">
+      <c r="A855" s="1" t="s">
+        <v>1241</v>
+      </c>
+    </row>
+    <row r="856" spans="1:18">
+      <c r="A856" s="1" t="s">
+        <v>1242</v>
+      </c>
+    </row>
+    <row r="857" spans="1:18">
+      <c r="A857" s="1" t="s">
+        <v>1243</v>
+      </c>
+    </row>
+    <row r="858" spans="1:18">
+      <c r="A858" s="1" t="s">
+        <v>1244</v>
+      </c>
+    </row>
+    <row r="859" spans="1:18">
+      <c r="A859" s="1" t="s">
+        <v>1244</v>
+      </c>
+    </row>
+    <row r="860" spans="1:18">
+      <c r="A860" s="1" t="s">
+        <v>1245</v>
+      </c>
+    </row>
+    <row r="861" spans="1:18">
+      <c r="A861" s="1" t="s">
+        <v>1246</v>
+      </c>
+    </row>
+    <row r="862" spans="1:18">
+      <c r="A862" s="1" t="s">
+        <v>1260</v>
+      </c>
+    </row>
+    <row r="863" spans="1:18">
+      <c r="A863" s="1" t="s">
+        <v>1247</v>
+      </c>
+    </row>
+    <row r="864" spans="1:18">
+      <c r="A864" s="1" t="s">
+        <v>1248</v>
+      </c>
+    </row>
+    <row r="865" spans="1:1">
+      <c r="A865" s="1" t="s">
+        <v>1261</v>
+      </c>
+    </row>
+    <row r="866" spans="1:1">
+      <c r="A866" s="1" t="s">
+        <v>1249</v>
+      </c>
+    </row>
+    <row r="867" spans="1:1">
+      <c r="A867" s="1" t="s">
+        <v>1250</v>
+      </c>
+    </row>
+    <row r="868" spans="1:1">
+      <c r="A868" s="1" t="s">
+        <v>1251</v>
+      </c>
+    </row>
+    <row r="869" spans="1:1">
+      <c r="A869" s="1" t="s">
+        <v>1252</v>
+      </c>
+    </row>
+    <row r="870" spans="1:1">
+      <c r="A870" s="1" t="s">
+        <v>1253</v>
+      </c>
+    </row>
+    <row r="871" spans="1:1">
+      <c r="A871" s="1" t="s">
+        <v>1254</v>
+      </c>
+    </row>
+    <row r="872" spans="1:1">
+      <c r="A872" s="1" t="s">
+        <v>1255</v>
+      </c>
+    </row>
+    <row r="873" spans="1:1">
+      <c r="A873" s="1" t="s">
+        <v>1256</v>
+      </c>
+    </row>
+    <row r="874" spans="1:1">
+      <c r="A874" s="1" t="s">
+        <v>1257</v>
+      </c>
+    </row>
+    <row r="875" spans="1:1">
+      <c r="A875" s="23" t="s">
+        <v>1258</v>
+      </c>
+    </row>
+    <row r="876" spans="1:1">
+      <c r="A876" s="23" t="s">
+        <v>1259</v>
+      </c>
+    </row>
+    <row r="877" spans="1:1">
+      <c r="A877" s="1" t="s">
+        <v>1262</v>
+      </c>
+    </row>
+    <row r="878" spans="1:1">
+      <c r="A878" s="1" t="s">
+        <v>1263</v>
+      </c>
+    </row>
+    <row r="879" spans="1:1">
+      <c r="A879" s="1" t="s">
+        <v>1264</v>
+      </c>
+    </row>
+    <row r="880" spans="1:1">
+      <c r="A880" s="1" t="s">
+        <v>1265</v>
+      </c>
+    </row>
+    <row r="881" spans="1:1">
+      <c r="A881" s="23" t="s">
+        <v>1266</v>
+      </c>
+    </row>
+    <row r="882" spans="1:1">
+      <c r="A882" s="23" t="s">
+        <v>1267</v>
+      </c>
+    </row>
+    <row r="883" spans="1:1">
+      <c r="A883" s="23" t="s">
+        <v>1268</v>
+      </c>
+    </row>
+    <row r="884" spans="1:1">
+      <c r="A884" s="23" t="s">
+        <v>1269</v>
+      </c>
+    </row>
+    <row r="885" spans="1:1">
+      <c r="A885" s="23" t="s">
+        <v>1270</v>
+      </c>
+    </row>
+    <row r="886" spans="1:1">
+      <c r="A886" s="23" t="s">
+        <v>1271</v>
+      </c>
+    </row>
+    <row r="887" spans="1:1">
+      <c r="A887" s="23" t="s">
+        <v>1272</v>
+      </c>
+    </row>
+    <row r="888" spans="1:1">
+      <c r="A888" s="23" t="s">
+        <v>1273</v>
+      </c>
+    </row>
+    <row r="889" spans="1:1">
+      <c r="A889" s="23" t="s">
+        <v>1274</v>
+      </c>
+    </row>
+    <row r="890" spans="1:1">
+      <c r="A890" s="23" t="s">
+        <v>1275</v>
+      </c>
+    </row>
+    <row r="891" spans="1:1">
+      <c r="A891" s="23" t="s">
+        <v>1276</v>
+      </c>
+    </row>
+    <row r="892" spans="1:1">
+      <c r="A892" s="23" t="s">
+        <v>1277</v>
+      </c>
+    </row>
+    <row r="893" spans="1:1">
+      <c r="A893" s="23" t="s">
+        <v>1278</v>
+      </c>
+    </row>
+    <row r="894" spans="1:1">
+      <c r="A894" s="23" t="s">
+        <v>1279</v>
+      </c>
+    </row>
+    <row r="895" spans="1:1">
+      <c r="A895" s="23" t="s">
+        <v>1280</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
P03697 to P03694 corrected in NCBI file
</commit_message>
<xml_diff>
--- a/source_data/pigs_samples_IDs_for_NCBI.xlsx
+++ b/source_data/pigs_samples_IDs_for_NCBI.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="28705"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="-460" windowWidth="28800" windowHeight="18000"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16000"/>
   </bookViews>
   <sheets>
     <sheet name="MIMARKS.survey.host-associated." sheetId="1" r:id="rId1"/>
@@ -355,7 +355,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15214" uniqueCount="1287">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15214" uniqueCount="1286">
   <si>
     <r>
       <rPr>
@@ -4189,9 +4189,6 @@
   </si>
   <si>
     <t>Ja30/319427</t>
-  </si>
-  <si>
-    <t>Ja30/P03697</t>
   </si>
   <si>
     <t>Ja30/316981</t>
@@ -5466,9 +5463,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AA892"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="M1" workbookViewId="0">
-      <pane ySplit="15" topLeftCell="A16" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="S35" sqref="S35"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="15" topLeftCell="A801" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A813" sqref="A813"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -5646,7 +5643,7 @@
         <v>37</v>
       </c>
       <c r="AA15" s="21" t="s">
-        <v>1219</v>
+        <v>1218</v>
       </c>
     </row>
     <row r="16" spans="1:27" ht="15">
@@ -6057,7 +6054,7 @@
     </row>
     <row r="23" spans="1:27" ht="15">
       <c r="A23" s="15" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
       <c r="B23"/>
       <c r="D23" s="1" t="s">
@@ -6113,7 +6110,7 @@
       </c>
       <c r="Z23"/>
       <c r="AA23" t="s">
-        <v>1217</v>
+        <v>1216</v>
       </c>
     </row>
     <row r="24" spans="1:27" ht="15">
@@ -8240,7 +8237,7 @@
     </row>
     <row r="61" spans="1:27" ht="15">
       <c r="A61" s="15" t="s">
-        <v>1221</v>
+        <v>1220</v>
       </c>
       <c r="B61"/>
       <c r="D61" s="1" t="s">
@@ -8295,7 +8292,7 @@
         <v>175</v>
       </c>
       <c r="AA61" t="s">
-        <v>1217</v>
+        <v>1216</v>
       </c>
     </row>
     <row r="62" spans="1:27" ht="15">
@@ -8471,7 +8468,7 @@
     </row>
     <row r="65" spans="1:27" ht="15">
       <c r="A65" s="15" t="s">
-        <v>1222</v>
+        <v>1221</v>
       </c>
       <c r="B65"/>
       <c r="D65" s="1" t="s">
@@ -8526,7 +8523,7 @@
         <v>175</v>
       </c>
       <c r="AA65" t="s">
-        <v>1217</v>
+        <v>1216</v>
       </c>
     </row>
     <row r="66" spans="1:27" ht="15">
@@ -10070,7 +10067,7 @@
     </row>
     <row r="93" spans="1:27" ht="15">
       <c r="A93" s="15" t="s">
-        <v>1223</v>
+        <v>1222</v>
       </c>
       <c r="B93"/>
       <c r="D93" s="1" t="s">
@@ -10125,7 +10122,7 @@
         <v>175</v>
       </c>
       <c r="AA93" t="s">
-        <v>1217</v>
+        <v>1216</v>
       </c>
     </row>
     <row r="94" spans="1:27" ht="15">
@@ -10643,7 +10640,7 @@
     </row>
     <row r="103" spans="1:27" ht="15">
       <c r="A103" s="15" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
       <c r="B103" s="22"/>
       <c r="C103" s="23"/>
@@ -10705,12 +10702,12 @@
       <c r="Y103" s="23"/>
       <c r="Z103" s="23"/>
       <c r="AA103" s="22" t="s">
-        <v>1218</v>
+        <v>1217</v>
       </c>
     </row>
     <row r="104" spans="1:27" ht="15">
       <c r="A104" s="15" t="s">
-        <v>1224</v>
+        <v>1223</v>
       </c>
       <c r="B104"/>
       <c r="D104" s="1" t="s">
@@ -10765,7 +10762,7 @@
         <v>175</v>
       </c>
       <c r="AA104" t="s">
-        <v>1217</v>
+        <v>1216</v>
       </c>
     </row>
     <row r="105" spans="1:27" ht="15">
@@ -12765,7 +12762,7 @@
     </row>
     <row r="140" spans="1:27" ht="15">
       <c r="A140" s="15" t="s">
-        <v>1222</v>
+        <v>1221</v>
       </c>
       <c r="B140" s="22"/>
       <c r="C140" s="23"/>
@@ -12827,12 +12824,12 @@
       <c r="Y140" s="23"/>
       <c r="Z140" s="23"/>
       <c r="AA140" s="22" t="s">
-        <v>1218</v>
+        <v>1217</v>
       </c>
     </row>
     <row r="141" spans="1:27" ht="15">
       <c r="A141" s="15" t="s">
-        <v>1223</v>
+        <v>1222</v>
       </c>
       <c r="B141" s="22"/>
       <c r="C141" s="23"/>
@@ -12894,12 +12891,12 @@
       <c r="Y141" s="23"/>
       <c r="Z141" s="23"/>
       <c r="AA141" s="22" t="s">
-        <v>1218</v>
+        <v>1217</v>
       </c>
     </row>
     <row r="142" spans="1:27" ht="15">
       <c r="A142" s="15" t="s">
-        <v>1226</v>
+        <v>1225</v>
       </c>
       <c r="B142" s="22"/>
       <c r="C142" s="23"/>
@@ -12961,12 +12958,12 @@
       <c r="Y142" s="23"/>
       <c r="Z142" s="22"/>
       <c r="AA142" s="22" t="s">
-        <v>1217</v>
+        <v>1216</v>
       </c>
     </row>
     <row r="143" spans="1:27" ht="15">
       <c r="A143" s="15" t="s">
-        <v>1227</v>
+        <v>1226</v>
       </c>
       <c r="B143" s="22"/>
       <c r="C143" s="23"/>
@@ -13028,12 +13025,12 @@
       <c r="Y143" s="23"/>
       <c r="Z143" s="23"/>
       <c r="AA143" s="22" t="s">
-        <v>1217</v>
+        <v>1216</v>
       </c>
     </row>
     <row r="144" spans="1:27" ht="15">
       <c r="A144" s="15" t="s">
-        <v>1225</v>
+        <v>1224</v>
       </c>
       <c r="B144"/>
       <c r="D144" s="1" t="s">
@@ -13088,12 +13085,12 @@
         <v>175</v>
       </c>
       <c r="AA144" t="s">
-        <v>1218</v>
+        <v>1217</v>
       </c>
     </row>
     <row r="145" spans="1:27" ht="15">
       <c r="A145" s="15" t="s">
-        <v>1229</v>
+        <v>1228</v>
       </c>
       <c r="B145"/>
       <c r="D145" s="1" t="s">
@@ -13148,12 +13145,12 @@
         <v>175</v>
       </c>
       <c r="AA145" t="s">
-        <v>1218</v>
+        <v>1217</v>
       </c>
     </row>
     <row r="146" spans="1:27" ht="15">
       <c r="A146" s="15" t="s">
-        <v>1227</v>
+        <v>1226</v>
       </c>
       <c r="B146"/>
       <c r="D146" s="1" t="s">
@@ -13208,12 +13205,12 @@
         <v>175</v>
       </c>
       <c r="AA146" t="s">
-        <v>1218</v>
+        <v>1217</v>
       </c>
     </row>
     <row r="147" spans="1:27" ht="15">
       <c r="A147" s="15" t="s">
-        <v>1230</v>
+        <v>1229</v>
       </c>
       <c r="B147"/>
       <c r="D147" s="1" t="s">
@@ -13268,12 +13265,12 @@
         <v>175</v>
       </c>
       <c r="AA147" t="s">
-        <v>1218</v>
+        <v>1217</v>
       </c>
     </row>
     <row r="148" spans="1:27" ht="15">
       <c r="A148" s="15" t="s">
-        <v>1228</v>
+        <v>1227</v>
       </c>
       <c r="B148"/>
       <c r="D148" s="1" t="s">
@@ -13328,7 +13325,7 @@
         <v>175</v>
       </c>
       <c r="AA148" t="s">
-        <v>1218</v>
+        <v>1217</v>
       </c>
     </row>
     <row r="149" spans="1:27" ht="15">
@@ -41131,7 +41128,7 @@
     </row>
     <row r="635" spans="1:24" ht="15">
       <c r="A635" s="15" t="s">
-        <v>1275</v>
+        <v>1274</v>
       </c>
       <c r="B635"/>
       <c r="D635" s="1" t="s">
@@ -50842,10 +50839,10 @@
         <v>174</v>
       </c>
       <c r="Q805" s="1" t="s">
+        <v>1214</v>
+      </c>
+      <c r="R805" s="1" t="s">
         <v>1215</v>
-      </c>
-      <c r="R805" s="1" t="s">
-        <v>1216</v>
       </c>
       <c r="X805" s="1" t="s">
         <v>175</v>
@@ -50889,10 +50886,10 @@
         <v>174</v>
       </c>
       <c r="Q806" s="1" t="s">
+        <v>1214</v>
+      </c>
+      <c r="R806" s="1" t="s">
         <v>1215</v>
-      </c>
-      <c r="R806" s="1" t="s">
-        <v>1216</v>
       </c>
       <c r="X806" s="1" t="s">
         <v>175</v>
@@ -50936,10 +50933,10 @@
         <v>174</v>
       </c>
       <c r="Q807" s="1" t="s">
+        <v>1214</v>
+      </c>
+      <c r="R807" s="1" t="s">
         <v>1215</v>
-      </c>
-      <c r="R807" s="1" t="s">
-        <v>1216</v>
       </c>
       <c r="X807" s="1" t="s">
         <v>175</v>
@@ -50983,10 +50980,10 @@
         <v>174</v>
       </c>
       <c r="Q808" s="1" t="s">
+        <v>1214</v>
+      </c>
+      <c r="R808" s="1" t="s">
         <v>1215</v>
-      </c>
-      <c r="R808" s="1" t="s">
-        <v>1216</v>
       </c>
       <c r="X808" s="1" t="s">
         <v>175</v>
@@ -51030,10 +51027,10 @@
         <v>174</v>
       </c>
       <c r="Q809" s="1" t="s">
+        <v>1214</v>
+      </c>
+      <c r="R809" s="1" t="s">
         <v>1215</v>
-      </c>
-      <c r="R809" s="1" t="s">
-        <v>1216</v>
       </c>
       <c r="X809" s="1" t="s">
         <v>175</v>
@@ -51077,10 +51074,10 @@
         <v>174</v>
       </c>
       <c r="Q810" s="1" t="s">
+        <v>1214</v>
+      </c>
+      <c r="R810" s="1" t="s">
         <v>1215</v>
-      </c>
-      <c r="R810" s="1" t="s">
-        <v>1216</v>
       </c>
       <c r="X810" s="1" t="s">
         <v>175</v>
@@ -51124,10 +51121,10 @@
         <v>174</v>
       </c>
       <c r="Q811" s="1" t="s">
+        <v>1214</v>
+      </c>
+      <c r="R811" s="1" t="s">
         <v>1215</v>
-      </c>
-      <c r="R811" s="1" t="s">
-        <v>1216</v>
       </c>
       <c r="X811" s="1" t="s">
         <v>175</v>
@@ -51135,7 +51132,7 @@
     </row>
     <row r="812" spans="1:24" ht="15">
       <c r="A812" s="16" t="s">
-        <v>1181</v>
+        <v>1276</v>
       </c>
       <c r="D812" s="1" t="s">
         <v>179</v>
@@ -51171,10 +51168,10 @@
         <v>174</v>
       </c>
       <c r="Q812" s="1" t="s">
+        <v>1214</v>
+      </c>
+      <c r="R812" s="1" t="s">
         <v>1215</v>
-      </c>
-      <c r="R812" s="1" t="s">
-        <v>1216</v>
       </c>
       <c r="X812" s="1" t="s">
         <v>175</v>
@@ -51182,7 +51179,7 @@
     </row>
     <row r="813" spans="1:24" ht="15">
       <c r="A813" s="16" t="s">
-        <v>1182</v>
+        <v>1181</v>
       </c>
       <c r="D813" s="1" t="s">
         <v>179</v>
@@ -51218,10 +51215,10 @@
         <v>174</v>
       </c>
       <c r="Q813" s="1" t="s">
+        <v>1214</v>
+      </c>
+      <c r="R813" s="1" t="s">
         <v>1215</v>
-      </c>
-      <c r="R813" s="1" t="s">
-        <v>1216</v>
       </c>
       <c r="X813" s="1" t="s">
         <v>175</v>
@@ -51229,7 +51226,7 @@
     </row>
     <row r="814" spans="1:24" ht="15">
       <c r="A814" s="16" t="s">
-        <v>1183</v>
+        <v>1182</v>
       </c>
       <c r="D814" s="1" t="s">
         <v>179</v>
@@ -51265,10 +51262,10 @@
         <v>174</v>
       </c>
       <c r="Q814" s="1" t="s">
+        <v>1214</v>
+      </c>
+      <c r="R814" s="1" t="s">
         <v>1215</v>
-      </c>
-      <c r="R814" s="1" t="s">
-        <v>1216</v>
       </c>
       <c r="X814" s="1" t="s">
         <v>175</v>
@@ -51276,7 +51273,7 @@
     </row>
     <row r="815" spans="1:24" ht="15">
       <c r="A815" s="16" t="s">
-        <v>1184</v>
+        <v>1183</v>
       </c>
       <c r="D815" s="1" t="s">
         <v>179</v>
@@ -51312,10 +51309,10 @@
         <v>174</v>
       </c>
       <c r="Q815" s="1" t="s">
+        <v>1214</v>
+      </c>
+      <c r="R815" s="1" t="s">
         <v>1215</v>
-      </c>
-      <c r="R815" s="1" t="s">
-        <v>1216</v>
       </c>
       <c r="X815" s="1" t="s">
         <v>175</v>
@@ -51323,7 +51320,7 @@
     </row>
     <row r="816" spans="1:24" ht="15">
       <c r="A816" s="16" t="s">
-        <v>1185</v>
+        <v>1184</v>
       </c>
       <c r="D816" s="1" t="s">
         <v>179</v>
@@ -51359,10 +51356,10 @@
         <v>174</v>
       </c>
       <c r="Q816" s="1" t="s">
+        <v>1214</v>
+      </c>
+      <c r="R816" s="1" t="s">
         <v>1215</v>
-      </c>
-      <c r="R816" s="1" t="s">
-        <v>1216</v>
       </c>
       <c r="X816" s="1" t="s">
         <v>175</v>
@@ -51370,7 +51367,7 @@
     </row>
     <row r="817" spans="1:24" ht="15">
       <c r="A817" s="16" t="s">
-        <v>1186</v>
+        <v>1185</v>
       </c>
       <c r="D817" s="1" t="s">
         <v>179</v>
@@ -51406,10 +51403,10 @@
         <v>174</v>
       </c>
       <c r="Q817" s="1" t="s">
+        <v>1214</v>
+      </c>
+      <c r="R817" s="1" t="s">
         <v>1215</v>
-      </c>
-      <c r="R817" s="1" t="s">
-        <v>1216</v>
       </c>
       <c r="X817" s="1" t="s">
         <v>175</v>
@@ -51417,7 +51414,7 @@
     </row>
     <row r="818" spans="1:24" ht="15">
       <c r="A818" s="16" t="s">
-        <v>1276</v>
+        <v>1275</v>
       </c>
       <c r="D818" s="1" t="s">
         <v>179</v>
@@ -51453,10 +51450,10 @@
         <v>174</v>
       </c>
       <c r="Q818" s="1" t="s">
+        <v>1214</v>
+      </c>
+      <c r="R818" s="1" t="s">
         <v>1215</v>
-      </c>
-      <c r="R818" s="1" t="s">
-        <v>1216</v>
       </c>
       <c r="X818" s="1" t="s">
         <v>175</v>
@@ -51464,7 +51461,7 @@
     </row>
     <row r="819" spans="1:24" ht="15">
       <c r="A819" s="16" t="s">
-        <v>1187</v>
+        <v>1186</v>
       </c>
       <c r="D819" s="1" t="s">
         <v>179</v>
@@ -51500,10 +51497,10 @@
         <v>174</v>
       </c>
       <c r="Q819" s="1" t="s">
+        <v>1214</v>
+      </c>
+      <c r="R819" s="1" t="s">
         <v>1215</v>
-      </c>
-      <c r="R819" s="1" t="s">
-        <v>1216</v>
       </c>
       <c r="X819" s="1" t="s">
         <v>175</v>
@@ -51511,7 +51508,7 @@
     </row>
     <row r="820" spans="1:24" ht="15">
       <c r="A820" s="16" t="s">
-        <v>1188</v>
+        <v>1187</v>
       </c>
       <c r="D820" s="1" t="s">
         <v>179</v>
@@ -51547,10 +51544,10 @@
         <v>174</v>
       </c>
       <c r="Q820" s="1" t="s">
+        <v>1214</v>
+      </c>
+      <c r="R820" s="1" t="s">
         <v>1215</v>
-      </c>
-      <c r="R820" s="1" t="s">
-        <v>1216</v>
       </c>
       <c r="X820" s="1" t="s">
         <v>175</v>
@@ -51558,7 +51555,7 @@
     </row>
     <row r="821" spans="1:24" ht="15">
       <c r="A821" s="16" t="s">
-        <v>1189</v>
+        <v>1188</v>
       </c>
       <c r="D821" s="1" t="s">
         <v>179</v>
@@ -51594,10 +51591,10 @@
         <v>174</v>
       </c>
       <c r="Q821" s="1" t="s">
+        <v>1214</v>
+      </c>
+      <c r="R821" s="1" t="s">
         <v>1215</v>
-      </c>
-      <c r="R821" s="1" t="s">
-        <v>1216</v>
       </c>
       <c r="X821" s="1" t="s">
         <v>175</v>
@@ -51605,7 +51602,7 @@
     </row>
     <row r="822" spans="1:24" ht="15">
       <c r="A822" s="16" t="s">
-        <v>1190</v>
+        <v>1189</v>
       </c>
       <c r="D822" s="1" t="s">
         <v>179</v>
@@ -51641,10 +51638,10 @@
         <v>174</v>
       </c>
       <c r="Q822" s="1" t="s">
+        <v>1214</v>
+      </c>
+      <c r="R822" s="1" t="s">
         <v>1215</v>
-      </c>
-      <c r="R822" s="1" t="s">
-        <v>1216</v>
       </c>
       <c r="X822" s="1" t="s">
         <v>175</v>
@@ -51652,7 +51649,7 @@
     </row>
     <row r="823" spans="1:24" ht="15">
       <c r="A823" s="16" t="s">
-        <v>1191</v>
+        <v>1190</v>
       </c>
       <c r="D823" s="1" t="s">
         <v>179</v>
@@ -51688,10 +51685,10 @@
         <v>174</v>
       </c>
       <c r="Q823" s="1" t="s">
+        <v>1214</v>
+      </c>
+      <c r="R823" s="1" t="s">
         <v>1215</v>
-      </c>
-      <c r="R823" s="1" t="s">
-        <v>1216</v>
       </c>
       <c r="X823" s="1" t="s">
         <v>175</v>
@@ -51699,7 +51696,7 @@
     </row>
     <row r="824" spans="1:24" ht="15">
       <c r="A824" s="16" t="s">
-        <v>1192</v>
+        <v>1191</v>
       </c>
       <c r="D824" s="1" t="s">
         <v>179</v>
@@ -51735,10 +51732,10 @@
         <v>174</v>
       </c>
       <c r="Q824" s="1" t="s">
+        <v>1214</v>
+      </c>
+      <c r="R824" s="1" t="s">
         <v>1215</v>
-      </c>
-      <c r="R824" s="1" t="s">
-        <v>1216</v>
       </c>
       <c r="X824" s="1" t="s">
         <v>175</v>
@@ -51746,7 +51743,7 @@
     </row>
     <row r="825" spans="1:24" ht="15">
       <c r="A825" s="16" t="s">
-        <v>1193</v>
+        <v>1192</v>
       </c>
       <c r="D825" s="1" t="s">
         <v>179</v>
@@ -51782,10 +51779,10 @@
         <v>174</v>
       </c>
       <c r="Q825" s="1" t="s">
+        <v>1214</v>
+      </c>
+      <c r="R825" s="1" t="s">
         <v>1215</v>
-      </c>
-      <c r="R825" s="1" t="s">
-        <v>1216</v>
       </c>
       <c r="X825" s="1" t="s">
         <v>175</v>
@@ -51793,7 +51790,7 @@
     </row>
     <row r="826" spans="1:24" ht="15">
       <c r="A826" s="16" t="s">
-        <v>1194</v>
+        <v>1193</v>
       </c>
       <c r="D826" s="1" t="s">
         <v>179</v>
@@ -51829,10 +51826,10 @@
         <v>174</v>
       </c>
       <c r="Q826" s="1" t="s">
+        <v>1214</v>
+      </c>
+      <c r="R826" s="1" t="s">
         <v>1215</v>
-      </c>
-      <c r="R826" s="1" t="s">
-        <v>1216</v>
       </c>
       <c r="X826" s="1" t="s">
         <v>175</v>
@@ -51840,7 +51837,7 @@
     </row>
     <row r="827" spans="1:24" ht="15">
       <c r="A827" s="16" t="s">
-        <v>1195</v>
+        <v>1194</v>
       </c>
       <c r="D827" s="1" t="s">
         <v>179</v>
@@ -51876,10 +51873,10 @@
         <v>174</v>
       </c>
       <c r="Q827" s="1" t="s">
+        <v>1214</v>
+      </c>
+      <c r="R827" s="1" t="s">
         <v>1215</v>
-      </c>
-      <c r="R827" s="1" t="s">
-        <v>1216</v>
       </c>
       <c r="X827" s="1" t="s">
         <v>175</v>
@@ -51887,7 +51884,7 @@
     </row>
     <row r="828" spans="1:24" ht="15">
       <c r="A828" s="16" t="s">
-        <v>1196</v>
+        <v>1195</v>
       </c>
       <c r="D828" s="1" t="s">
         <v>179</v>
@@ -51923,10 +51920,10 @@
         <v>174</v>
       </c>
       <c r="Q828" s="1" t="s">
+        <v>1214</v>
+      </c>
+      <c r="R828" s="1" t="s">
         <v>1215</v>
-      </c>
-      <c r="R828" s="1" t="s">
-        <v>1216</v>
       </c>
       <c r="X828" s="1" t="s">
         <v>175</v>
@@ -51934,7 +51931,7 @@
     </row>
     <row r="829" spans="1:24" ht="15">
       <c r="A829" s="16" t="s">
-        <v>1197</v>
+        <v>1196</v>
       </c>
       <c r="D829" s="1" t="s">
         <v>179</v>
@@ -51970,10 +51967,10 @@
         <v>174</v>
       </c>
       <c r="Q829" s="1" t="s">
+        <v>1214</v>
+      </c>
+      <c r="R829" s="1" t="s">
         <v>1215</v>
-      </c>
-      <c r="R829" s="1" t="s">
-        <v>1216</v>
       </c>
       <c r="X829" s="1" t="s">
         <v>175</v>
@@ -51981,7 +51978,7 @@
     </row>
     <row r="830" spans="1:24" ht="15">
       <c r="A830" s="16" t="s">
-        <v>1198</v>
+        <v>1197</v>
       </c>
       <c r="D830" s="1" t="s">
         <v>179</v>
@@ -52017,10 +52014,10 @@
         <v>174</v>
       </c>
       <c r="Q830" s="1" t="s">
+        <v>1214</v>
+      </c>
+      <c r="R830" s="1" t="s">
         <v>1215</v>
-      </c>
-      <c r="R830" s="1" t="s">
-        <v>1216</v>
       </c>
       <c r="X830" s="1" t="s">
         <v>175</v>
@@ -52028,7 +52025,7 @@
     </row>
     <row r="831" spans="1:24" ht="15">
       <c r="A831" s="16" t="s">
-        <v>1199</v>
+        <v>1198</v>
       </c>
       <c r="D831" s="1" t="s">
         <v>179</v>
@@ -52064,10 +52061,10 @@
         <v>174</v>
       </c>
       <c r="Q831" s="1" t="s">
+        <v>1214</v>
+      </c>
+      <c r="R831" s="1" t="s">
         <v>1215</v>
-      </c>
-      <c r="R831" s="1" t="s">
-        <v>1216</v>
       </c>
       <c r="X831" s="1" t="s">
         <v>175</v>
@@ -52075,7 +52072,7 @@
     </row>
     <row r="832" spans="1:24" ht="15">
       <c r="A832" s="16" t="s">
-        <v>1200</v>
+        <v>1199</v>
       </c>
       <c r="D832" s="1" t="s">
         <v>179</v>
@@ -52111,10 +52108,10 @@
         <v>174</v>
       </c>
       <c r="Q832" s="1" t="s">
+        <v>1214</v>
+      </c>
+      <c r="R832" s="1" t="s">
         <v>1215</v>
-      </c>
-      <c r="R832" s="1" t="s">
-        <v>1216</v>
       </c>
       <c r="X832" s="1" t="s">
         <v>175</v>
@@ -52122,7 +52119,7 @@
     </row>
     <row r="833" spans="1:24" ht="15">
       <c r="A833" s="16" t="s">
-        <v>1201</v>
+        <v>1200</v>
       </c>
       <c r="D833" s="1" t="s">
         <v>179</v>
@@ -52158,10 +52155,10 @@
         <v>174</v>
       </c>
       <c r="Q833" s="1" t="s">
+        <v>1214</v>
+      </c>
+      <c r="R833" s="1" t="s">
         <v>1215</v>
-      </c>
-      <c r="R833" s="1" t="s">
-        <v>1216</v>
       </c>
       <c r="X833" s="1" t="s">
         <v>175</v>
@@ -52169,7 +52166,7 @@
     </row>
     <row r="834" spans="1:24" ht="15">
       <c r="A834" s="16" t="s">
-        <v>1202</v>
+        <v>1201</v>
       </c>
       <c r="D834" s="1" t="s">
         <v>179</v>
@@ -52205,10 +52202,10 @@
         <v>174</v>
       </c>
       <c r="Q834" s="1" t="s">
+        <v>1214</v>
+      </c>
+      <c r="R834" s="1" t="s">
         <v>1215</v>
-      </c>
-      <c r="R834" s="1" t="s">
-        <v>1216</v>
       </c>
       <c r="X834" s="1" t="s">
         <v>175</v>
@@ -52216,7 +52213,7 @@
     </row>
     <row r="835" spans="1:24" ht="15">
       <c r="A835" s="16" t="s">
-        <v>1203</v>
+        <v>1202</v>
       </c>
       <c r="D835" s="1" t="s">
         <v>179</v>
@@ -52252,10 +52249,10 @@
         <v>174</v>
       </c>
       <c r="Q835" s="1" t="s">
+        <v>1214</v>
+      </c>
+      <c r="R835" s="1" t="s">
         <v>1215</v>
-      </c>
-      <c r="R835" s="1" t="s">
-        <v>1216</v>
       </c>
       <c r="X835" s="1" t="s">
         <v>175</v>
@@ -52263,7 +52260,7 @@
     </row>
     <row r="836" spans="1:24" ht="15">
       <c r="A836" s="16" t="s">
-        <v>1204</v>
+        <v>1203</v>
       </c>
       <c r="D836" s="1" t="s">
         <v>179</v>
@@ -52299,10 +52296,10 @@
         <v>174</v>
       </c>
       <c r="Q836" s="1" t="s">
+        <v>1214</v>
+      </c>
+      <c r="R836" s="1" t="s">
         <v>1215</v>
-      </c>
-      <c r="R836" s="1" t="s">
-        <v>1216</v>
       </c>
       <c r="X836" s="1" t="s">
         <v>175</v>
@@ -52310,7 +52307,7 @@
     </row>
     <row r="837" spans="1:24" ht="15">
       <c r="A837" s="16" t="s">
-        <v>1205</v>
+        <v>1204</v>
       </c>
       <c r="D837" s="1" t="s">
         <v>179</v>
@@ -52346,10 +52343,10 @@
         <v>174</v>
       </c>
       <c r="Q837" s="1" t="s">
+        <v>1214</v>
+      </c>
+      <c r="R837" s="1" t="s">
         <v>1215</v>
-      </c>
-      <c r="R837" s="1" t="s">
-        <v>1216</v>
       </c>
       <c r="X837" s="1" t="s">
         <v>175</v>
@@ -52357,7 +52354,7 @@
     </row>
     <row r="838" spans="1:24" ht="15">
       <c r="A838" s="16" t="s">
-        <v>1206</v>
+        <v>1205</v>
       </c>
       <c r="D838" s="1" t="s">
         <v>179</v>
@@ -52393,10 +52390,10 @@
         <v>174</v>
       </c>
       <c r="Q838" s="1" t="s">
+        <v>1214</v>
+      </c>
+      <c r="R838" s="1" t="s">
         <v>1215</v>
-      </c>
-      <c r="R838" s="1" t="s">
-        <v>1216</v>
       </c>
       <c r="X838" s="1" t="s">
         <v>175</v>
@@ -52404,7 +52401,7 @@
     </row>
     <row r="839" spans="1:24" ht="15">
       <c r="A839" s="16" t="s">
-        <v>1207</v>
+        <v>1206</v>
       </c>
       <c r="D839" s="1" t="s">
         <v>179</v>
@@ -52440,10 +52437,10 @@
         <v>174</v>
       </c>
       <c r="Q839" s="1" t="s">
+        <v>1214</v>
+      </c>
+      <c r="R839" s="1" t="s">
         <v>1215</v>
-      </c>
-      <c r="R839" s="1" t="s">
-        <v>1216</v>
       </c>
       <c r="X839" s="1" t="s">
         <v>175</v>
@@ -52451,7 +52448,7 @@
     </row>
     <row r="840" spans="1:24" ht="15">
       <c r="A840" s="16" t="s">
-        <v>1208</v>
+        <v>1207</v>
       </c>
       <c r="D840" s="1" t="s">
         <v>179</v>
@@ -52487,10 +52484,10 @@
         <v>174</v>
       </c>
       <c r="Q840" s="1" t="s">
+        <v>1214</v>
+      </c>
+      <c r="R840" s="1" t="s">
         <v>1215</v>
-      </c>
-      <c r="R840" s="1" t="s">
-        <v>1216</v>
       </c>
       <c r="X840" s="1" t="s">
         <v>175</v>
@@ -52498,7 +52495,7 @@
     </row>
     <row r="841" spans="1:24" ht="15">
       <c r="A841" s="16" t="s">
-        <v>1209</v>
+        <v>1208</v>
       </c>
       <c r="D841" s="1" t="s">
         <v>179</v>
@@ -52534,10 +52531,10 @@
         <v>174</v>
       </c>
       <c r="Q841" s="1" t="s">
+        <v>1214</v>
+      </c>
+      <c r="R841" s="1" t="s">
         <v>1215</v>
-      </c>
-      <c r="R841" s="1" t="s">
-        <v>1216</v>
       </c>
       <c r="X841" s="1" t="s">
         <v>175</v>
@@ -52545,7 +52542,7 @@
     </row>
     <row r="842" spans="1:24" ht="15">
       <c r="A842" s="16" t="s">
-        <v>1210</v>
+        <v>1209</v>
       </c>
       <c r="D842" s="1" t="s">
         <v>179</v>
@@ -52581,10 +52578,10 @@
         <v>174</v>
       </c>
       <c r="Q842" s="1" t="s">
+        <v>1214</v>
+      </c>
+      <c r="R842" s="1" t="s">
         <v>1215</v>
-      </c>
-      <c r="R842" s="1" t="s">
-        <v>1216</v>
       </c>
       <c r="X842" s="1" t="s">
         <v>175</v>
@@ -52592,7 +52589,7 @@
     </row>
     <row r="843" spans="1:24" ht="15">
       <c r="A843" s="16" t="s">
-        <v>1211</v>
+        <v>1210</v>
       </c>
       <c r="D843" s="1" t="s">
         <v>179</v>
@@ -52628,10 +52625,10 @@
         <v>174</v>
       </c>
       <c r="Q843" s="1" t="s">
+        <v>1214</v>
+      </c>
+      <c r="R843" s="1" t="s">
         <v>1215</v>
-      </c>
-      <c r="R843" s="1" t="s">
-        <v>1216</v>
       </c>
       <c r="X843" s="1" t="s">
         <v>175</v>
@@ -52639,7 +52636,7 @@
     </row>
     <row r="844" spans="1:24" ht="15">
       <c r="A844" s="16" t="s">
-        <v>1212</v>
+        <v>1211</v>
       </c>
       <c r="D844" s="1" t="s">
         <v>179</v>
@@ -52675,10 +52672,10 @@
         <v>174</v>
       </c>
       <c r="Q844" s="1" t="s">
+        <v>1214</v>
+      </c>
+      <c r="R844" s="1" t="s">
         <v>1215</v>
-      </c>
-      <c r="R844" s="1" t="s">
-        <v>1216</v>
       </c>
       <c r="X844" s="1" t="s">
         <v>175</v>
@@ -52686,7 +52683,7 @@
     </row>
     <row r="845" spans="1:24" ht="15">
       <c r="A845" s="16" t="s">
-        <v>1213</v>
+        <v>1212</v>
       </c>
       <c r="D845" s="1" t="s">
         <v>179</v>
@@ -52722,10 +52719,10 @@
         <v>174</v>
       </c>
       <c r="Q845" s="1" t="s">
+        <v>1214</v>
+      </c>
+      <c r="R845" s="1" t="s">
         <v>1215</v>
-      </c>
-      <c r="R845" s="1" t="s">
-        <v>1216</v>
       </c>
       <c r="X845" s="1" t="s">
         <v>175</v>
@@ -52733,7 +52730,7 @@
     </row>
     <row r="846" spans="1:24" ht="15">
       <c r="A846" s="16" t="s">
-        <v>1214</v>
+        <v>1213</v>
       </c>
       <c r="D846" s="1" t="s">
         <v>179</v>
@@ -52769,10 +52766,10 @@
         <v>174</v>
       </c>
       <c r="Q846" s="1" t="s">
+        <v>1214</v>
+      </c>
+      <c r="R846" s="1" t="s">
         <v>1215</v>
-      </c>
-      <c r="R846" s="1" t="s">
-        <v>1216</v>
       </c>
       <c r="X846" s="1" t="s">
         <v>175</v>
@@ -52780,7 +52777,7 @@
     </row>
     <row r="847" spans="1:24" ht="15">
       <c r="A847" s="16" t="s">
-        <v>1277</v>
+        <v>1276</v>
       </c>
       <c r="D847" s="1" t="s">
         <v>179</v>
@@ -52816,10 +52813,10 @@
         <v>174</v>
       </c>
       <c r="Q847" s="1" t="s">
+        <v>1214</v>
+      </c>
+      <c r="R847" s="1" t="s">
         <v>1215</v>
-      </c>
-      <c r="R847" s="1" t="s">
-        <v>1216</v>
       </c>
       <c r="X847" s="1" t="s">
         <v>175</v>
@@ -52827,49 +52824,49 @@
     </row>
     <row r="848" spans="1:24" ht="15">
       <c r="A848" s="1" t="s">
-        <v>1231</v>
+        <v>1230</v>
       </c>
       <c r="D848" s="1" t="s">
-        <v>1279</v>
+        <v>1278</v>
       </c>
       <c r="E848" s="17">
         <v>42961</v>
       </c>
       <c r="F848" s="1" t="s">
+        <v>1280</v>
+      </c>
+      <c r="G848" s="1" t="s">
         <v>1281</v>
       </c>
-      <c r="G848" s="1" t="s">
-        <v>1282</v>
-      </c>
       <c r="H848" s="1" t="s">
-        <v>1282</v>
+        <v>1281</v>
       </c>
       <c r="I848" s="1" t="s">
         <v>169</v>
       </c>
       <c r="J848" s="1" t="s">
-        <v>1280</v>
+        <v>1279</v>
       </c>
       <c r="K848" s="9" t="s">
-        <v>1286</v>
+        <v>1285</v>
       </c>
       <c r="M848" s="1" t="s">
         <v>954</v>
       </c>
       <c r="N848" s="1" t="s">
-        <v>1280</v>
+        <v>1279</v>
       </c>
       <c r="O848" s="1" t="s">
-        <v>1280</v>
+        <v>1279</v>
       </c>
       <c r="P848" s="1" t="s">
-        <v>1280</v>
+        <v>1279</v>
       </c>
       <c r="Q848" s="1" t="s">
-        <v>1280</v>
+        <v>1279</v>
       </c>
       <c r="S848" s="1" t="s">
-        <v>1280</v>
+        <v>1279</v>
       </c>
       <c r="X848" s="1" t="s">
         <v>175</v>
@@ -52877,49 +52874,49 @@
     </row>
     <row r="849" spans="1:24" ht="15">
       <c r="A849" s="1" t="s">
-        <v>1232</v>
+        <v>1231</v>
       </c>
       <c r="D849" s="1" t="s">
-        <v>1279</v>
+        <v>1278</v>
       </c>
       <c r="E849" s="17">
         <v>42961</v>
       </c>
       <c r="F849" s="1" t="s">
+        <v>1280</v>
+      </c>
+      <c r="G849" s="1" t="s">
         <v>1281</v>
       </c>
-      <c r="G849" s="1" t="s">
-        <v>1282</v>
-      </c>
       <c r="H849" s="1" t="s">
-        <v>1282</v>
+        <v>1281</v>
       </c>
       <c r="I849" s="1" t="s">
         <v>169</v>
       </c>
       <c r="J849" s="1" t="s">
-        <v>1280</v>
+        <v>1279</v>
       </c>
       <c r="K849" s="9" t="s">
-        <v>1286</v>
+        <v>1285</v>
       </c>
       <c r="M849" s="1" t="s">
         <v>954</v>
       </c>
       <c r="N849" s="1" t="s">
-        <v>1280</v>
+        <v>1279</v>
       </c>
       <c r="O849" s="1" t="s">
-        <v>1280</v>
+        <v>1279</v>
       </c>
       <c r="P849" s="1" t="s">
-        <v>1280</v>
+        <v>1279</v>
       </c>
       <c r="Q849" s="1" t="s">
-        <v>1280</v>
+        <v>1279</v>
       </c>
       <c r="S849" s="1" t="s">
-        <v>1280</v>
+        <v>1279</v>
       </c>
       <c r="X849" s="1" t="s">
         <v>175</v>
@@ -52927,49 +52924,49 @@
     </row>
     <row r="850" spans="1:24" ht="15">
       <c r="A850" s="1" t="s">
-        <v>1233</v>
+        <v>1232</v>
       </c>
       <c r="D850" s="1" t="s">
-        <v>1279</v>
+        <v>1278</v>
       </c>
       <c r="E850" s="17">
         <v>42961</v>
       </c>
       <c r="F850" s="1" t="s">
+        <v>1280</v>
+      </c>
+      <c r="G850" s="1" t="s">
         <v>1281</v>
       </c>
-      <c r="G850" s="1" t="s">
-        <v>1282</v>
-      </c>
       <c r="H850" s="1" t="s">
-        <v>1282</v>
+        <v>1281</v>
       </c>
       <c r="I850" s="1" t="s">
         <v>169</v>
       </c>
       <c r="J850" s="1" t="s">
-        <v>1280</v>
+        <v>1279</v>
       </c>
       <c r="K850" s="9" t="s">
-        <v>1286</v>
+        <v>1285</v>
       </c>
       <c r="M850" s="1" t="s">
         <v>954</v>
       </c>
       <c r="N850" s="1" t="s">
-        <v>1280</v>
+        <v>1279</v>
       </c>
       <c r="O850" s="1" t="s">
-        <v>1280</v>
+        <v>1279</v>
       </c>
       <c r="P850" s="1" t="s">
-        <v>1280</v>
+        <v>1279</v>
       </c>
       <c r="Q850" s="1" t="s">
-        <v>1280</v>
+        <v>1279</v>
       </c>
       <c r="S850" s="1" t="s">
-        <v>1280</v>
+        <v>1279</v>
       </c>
       <c r="X850" s="1" t="s">
         <v>175</v>
@@ -52977,49 +52974,49 @@
     </row>
     <row r="851" spans="1:24" ht="15">
       <c r="A851" s="1" t="s">
-        <v>1234</v>
+        <v>1233</v>
       </c>
       <c r="D851" s="1" t="s">
-        <v>1279</v>
+        <v>1278</v>
       </c>
       <c r="E851" s="17">
         <v>42961</v>
       </c>
       <c r="F851" s="1" t="s">
+        <v>1280</v>
+      </c>
+      <c r="G851" s="1" t="s">
         <v>1281</v>
       </c>
-      <c r="G851" s="1" t="s">
-        <v>1282</v>
-      </c>
       <c r="H851" s="1" t="s">
-        <v>1282</v>
+        <v>1281</v>
       </c>
       <c r="I851" s="1" t="s">
         <v>169</v>
       </c>
       <c r="J851" s="1" t="s">
-        <v>1280</v>
+        <v>1279</v>
       </c>
       <c r="K851" s="9" t="s">
-        <v>1286</v>
+        <v>1285</v>
       </c>
       <c r="M851" s="1" t="s">
         <v>954</v>
       </c>
       <c r="N851" s="1" t="s">
-        <v>1280</v>
+        <v>1279</v>
       </c>
       <c r="O851" s="1" t="s">
-        <v>1280</v>
+        <v>1279</v>
       </c>
       <c r="P851" s="1" t="s">
-        <v>1280</v>
+        <v>1279</v>
       </c>
       <c r="Q851" s="1" t="s">
-        <v>1280</v>
+        <v>1279</v>
       </c>
       <c r="S851" s="1" t="s">
-        <v>1280</v>
+        <v>1279</v>
       </c>
       <c r="X851" s="1" t="s">
         <v>175</v>
@@ -53027,49 +53024,49 @@
     </row>
     <row r="852" spans="1:24" ht="15">
       <c r="A852" s="1" t="s">
-        <v>1235</v>
+        <v>1234</v>
       </c>
       <c r="D852" s="1" t="s">
-        <v>1279</v>
+        <v>1278</v>
       </c>
       <c r="E852" s="17">
         <v>42961</v>
       </c>
       <c r="F852" s="1" t="s">
+        <v>1280</v>
+      </c>
+      <c r="G852" s="1" t="s">
         <v>1281</v>
       </c>
-      <c r="G852" s="1" t="s">
-        <v>1282</v>
-      </c>
       <c r="H852" s="1" t="s">
-        <v>1282</v>
+        <v>1281</v>
       </c>
       <c r="I852" s="1" t="s">
         <v>169</v>
       </c>
       <c r="J852" s="1" t="s">
-        <v>1280</v>
+        <v>1279</v>
       </c>
       <c r="K852" s="9" t="s">
-        <v>1286</v>
+        <v>1285</v>
       </c>
       <c r="M852" s="1" t="s">
         <v>954</v>
       </c>
       <c r="N852" s="1" t="s">
-        <v>1280</v>
+        <v>1279</v>
       </c>
       <c r="O852" s="1" t="s">
-        <v>1280</v>
+        <v>1279</v>
       </c>
       <c r="P852" s="1" t="s">
-        <v>1280</v>
+        <v>1279</v>
       </c>
       <c r="Q852" s="1" t="s">
-        <v>1280</v>
+        <v>1279</v>
       </c>
       <c r="S852" s="1" t="s">
-        <v>1280</v>
+        <v>1279</v>
       </c>
       <c r="X852" s="1" t="s">
         <v>175</v>
@@ -53077,49 +53074,49 @@
     </row>
     <row r="853" spans="1:24" ht="15">
       <c r="A853" s="1" t="s">
-        <v>1236</v>
+        <v>1235</v>
       </c>
       <c r="D853" s="1" t="s">
-        <v>1279</v>
+        <v>1278</v>
       </c>
       <c r="E853" s="17">
         <v>42961</v>
       </c>
       <c r="F853" s="1" t="s">
+        <v>1280</v>
+      </c>
+      <c r="G853" s="1" t="s">
         <v>1281</v>
       </c>
-      <c r="G853" s="1" t="s">
-        <v>1282</v>
-      </c>
       <c r="H853" s="1" t="s">
-        <v>1282</v>
+        <v>1281</v>
       </c>
       <c r="I853" s="1" t="s">
         <v>169</v>
       </c>
       <c r="J853" s="1" t="s">
-        <v>1280</v>
+        <v>1279</v>
       </c>
       <c r="K853" s="9" t="s">
-        <v>1286</v>
+        <v>1285</v>
       </c>
       <c r="M853" s="1" t="s">
         <v>954</v>
       </c>
       <c r="N853" s="1" t="s">
-        <v>1280</v>
+        <v>1279</v>
       </c>
       <c r="O853" s="1" t="s">
-        <v>1280</v>
+        <v>1279</v>
       </c>
       <c r="P853" s="1" t="s">
-        <v>1280</v>
+        <v>1279</v>
       </c>
       <c r="Q853" s="1" t="s">
-        <v>1280</v>
+        <v>1279</v>
       </c>
       <c r="S853" s="1" t="s">
-        <v>1280</v>
+        <v>1279</v>
       </c>
       <c r="X853" s="1" t="s">
         <v>175</v>
@@ -53127,49 +53124,49 @@
     </row>
     <row r="854" spans="1:24" ht="15">
       <c r="A854" s="1" t="s">
-        <v>1237</v>
+        <v>1236</v>
       </c>
       <c r="D854" s="1" t="s">
-        <v>1279</v>
+        <v>1278</v>
       </c>
       <c r="E854" s="17">
         <v>42961</v>
       </c>
       <c r="F854" s="1" t="s">
+        <v>1280</v>
+      </c>
+      <c r="G854" s="1" t="s">
         <v>1281</v>
       </c>
-      <c r="G854" s="1" t="s">
-        <v>1282</v>
-      </c>
       <c r="H854" s="1" t="s">
-        <v>1282</v>
+        <v>1281</v>
       </c>
       <c r="I854" s="1" t="s">
         <v>169</v>
       </c>
       <c r="J854" s="1" t="s">
-        <v>1280</v>
+        <v>1279</v>
       </c>
       <c r="K854" s="9" t="s">
-        <v>1286</v>
+        <v>1285</v>
       </c>
       <c r="M854" s="1" t="s">
         <v>954</v>
       </c>
       <c r="N854" s="1" t="s">
-        <v>1280</v>
+        <v>1279</v>
       </c>
       <c r="O854" s="1" t="s">
-        <v>1280</v>
+        <v>1279</v>
       </c>
       <c r="P854" s="1" t="s">
-        <v>1280</v>
+        <v>1279</v>
       </c>
       <c r="Q854" s="1" t="s">
-        <v>1280</v>
+        <v>1279</v>
       </c>
       <c r="S854" s="1" t="s">
-        <v>1280</v>
+        <v>1279</v>
       </c>
       <c r="X854" s="1" t="s">
         <v>175</v>
@@ -53177,49 +53174,49 @@
     </row>
     <row r="855" spans="1:24" ht="15">
       <c r="A855" s="1" t="s">
-        <v>1238</v>
+        <v>1237</v>
       </c>
       <c r="D855" s="1" t="s">
-        <v>1279</v>
+        <v>1278</v>
       </c>
       <c r="E855" s="17">
         <v>42961</v>
       </c>
       <c r="F855" s="1" t="s">
+        <v>1280</v>
+      </c>
+      <c r="G855" s="1" t="s">
         <v>1281</v>
       </c>
-      <c r="G855" s="1" t="s">
-        <v>1282</v>
-      </c>
       <c r="H855" s="1" t="s">
-        <v>1282</v>
+        <v>1281</v>
       </c>
       <c r="I855" s="1" t="s">
         <v>169</v>
       </c>
       <c r="J855" s="1" t="s">
-        <v>1280</v>
+        <v>1279</v>
       </c>
       <c r="K855" s="9" t="s">
-        <v>1286</v>
+        <v>1285</v>
       </c>
       <c r="M855" s="1" t="s">
         <v>954</v>
       </c>
       <c r="N855" s="1" t="s">
-        <v>1280</v>
+        <v>1279</v>
       </c>
       <c r="O855" s="1" t="s">
-        <v>1280</v>
+        <v>1279</v>
       </c>
       <c r="P855" s="1" t="s">
-        <v>1280</v>
+        <v>1279</v>
       </c>
       <c r="Q855" s="1" t="s">
-        <v>1280</v>
+        <v>1279</v>
       </c>
       <c r="S855" s="1" t="s">
-        <v>1280</v>
+        <v>1279</v>
       </c>
       <c r="X855" s="1" t="s">
         <v>175</v>
@@ -53227,49 +53224,49 @@
     </row>
     <row r="856" spans="1:24" ht="15">
       <c r="A856" s="1" t="s">
-        <v>1238</v>
+        <v>1237</v>
       </c>
       <c r="D856" s="1" t="s">
-        <v>1279</v>
+        <v>1278</v>
       </c>
       <c r="E856" s="17">
         <v>42961</v>
       </c>
       <c r="F856" s="1" t="s">
+        <v>1280</v>
+      </c>
+      <c r="G856" s="1" t="s">
         <v>1281</v>
       </c>
-      <c r="G856" s="1" t="s">
-        <v>1282</v>
-      </c>
       <c r="H856" s="1" t="s">
-        <v>1282</v>
+        <v>1281</v>
       </c>
       <c r="I856" s="1" t="s">
         <v>169</v>
       </c>
       <c r="J856" s="1" t="s">
-        <v>1280</v>
+        <v>1279</v>
       </c>
       <c r="K856" s="9" t="s">
-        <v>1286</v>
+        <v>1285</v>
       </c>
       <c r="M856" s="1" t="s">
         <v>954</v>
       </c>
       <c r="N856" s="1" t="s">
-        <v>1280</v>
+        <v>1279</v>
       </c>
       <c r="O856" s="1" t="s">
-        <v>1280</v>
+        <v>1279</v>
       </c>
       <c r="P856" s="1" t="s">
-        <v>1280</v>
+        <v>1279</v>
       </c>
       <c r="Q856" s="1" t="s">
-        <v>1280</v>
+        <v>1279</v>
       </c>
       <c r="S856" s="1" t="s">
-        <v>1280</v>
+        <v>1279</v>
       </c>
       <c r="X856" s="1" t="s">
         <v>175</v>
@@ -53277,49 +53274,49 @@
     </row>
     <row r="857" spans="1:24" ht="15">
       <c r="A857" s="1" t="s">
-        <v>1239</v>
+        <v>1238</v>
       </c>
       <c r="D857" s="1" t="s">
-        <v>1279</v>
+        <v>1278</v>
       </c>
       <c r="E857" s="17">
         <v>42961</v>
       </c>
       <c r="F857" s="1" t="s">
+        <v>1280</v>
+      </c>
+      <c r="G857" s="1" t="s">
         <v>1281</v>
       </c>
-      <c r="G857" s="1" t="s">
-        <v>1282</v>
-      </c>
       <c r="H857" s="1" t="s">
-        <v>1282</v>
+        <v>1281</v>
       </c>
       <c r="I857" s="1" t="s">
         <v>169</v>
       </c>
       <c r="J857" s="1" t="s">
-        <v>1280</v>
+        <v>1279</v>
       </c>
       <c r="K857" s="9" t="s">
-        <v>1286</v>
+        <v>1285</v>
       </c>
       <c r="M857" s="1" t="s">
         <v>954</v>
       </c>
       <c r="N857" s="1" t="s">
-        <v>1280</v>
+        <v>1279</v>
       </c>
       <c r="O857" s="1" t="s">
-        <v>1280</v>
+        <v>1279</v>
       </c>
       <c r="P857" s="1" t="s">
-        <v>1280</v>
+        <v>1279</v>
       </c>
       <c r="Q857" s="1" t="s">
-        <v>1280</v>
+        <v>1279</v>
       </c>
       <c r="S857" s="1" t="s">
-        <v>1280</v>
+        <v>1279</v>
       </c>
       <c r="X857" s="1" t="s">
         <v>175</v>
@@ -53327,28 +53324,28 @@
     </row>
     <row r="858" spans="1:24" ht="15">
       <c r="A858" s="1" t="s">
-        <v>1240</v>
+        <v>1239</v>
       </c>
       <c r="D858" s="1" t="s">
-        <v>1278</v>
+        <v>1277</v>
       </c>
       <c r="E858" s="17">
         <v>43124</v>
       </c>
       <c r="F858" s="1" t="s">
-        <v>1281</v>
+        <v>1280</v>
       </c>
       <c r="G858" s="1" t="s">
-        <v>1283</v>
+        <v>1282</v>
       </c>
       <c r="H858" s="1" t="s">
-        <v>1283</v>
+        <v>1282</v>
       </c>
       <c r="I858" s="1" t="s">
         <v>169</v>
       </c>
       <c r="J858" s="1" t="s">
-        <v>1280</v>
+        <v>1279</v>
       </c>
       <c r="K858" s="9" t="s">
         <v>170</v>
@@ -53357,19 +53354,19 @@
         <v>954</v>
       </c>
       <c r="N858" s="1" t="s">
-        <v>1280</v>
+        <v>1279</v>
       </c>
       <c r="O858" s="1" t="s">
-        <v>1280</v>
+        <v>1279</v>
       </c>
       <c r="P858" s="1" t="s">
-        <v>1280</v>
+        <v>1279</v>
       </c>
       <c r="Q858" s="1" t="s">
-        <v>1280</v>
+        <v>1279</v>
       </c>
       <c r="S858" s="1" t="s">
-        <v>1280</v>
+        <v>1279</v>
       </c>
       <c r="X858" s="1" t="s">
         <v>175</v>
@@ -53377,28 +53374,28 @@
     </row>
     <row r="859" spans="1:24" ht="15">
       <c r="A859" s="1" t="s">
-        <v>1254</v>
+        <v>1253</v>
       </c>
       <c r="D859" s="1" t="s">
-        <v>1278</v>
+        <v>1277</v>
       </c>
       <c r="E859" s="17">
         <v>43124</v>
       </c>
       <c r="F859" s="1" t="s">
-        <v>1281</v>
+        <v>1280</v>
       </c>
       <c r="G859" s="1" t="s">
-        <v>1284</v>
+        <v>1283</v>
       </c>
       <c r="H859" s="1" t="s">
-        <v>1284</v>
+        <v>1283</v>
       </c>
       <c r="I859" s="1" t="s">
         <v>169</v>
       </c>
       <c r="J859" s="1" t="s">
-        <v>1280</v>
+        <v>1279</v>
       </c>
       <c r="K859" s="9" t="s">
         <v>170</v>
@@ -53407,19 +53404,19 @@
         <v>954</v>
       </c>
       <c r="N859" s="1" t="s">
-        <v>1280</v>
+        <v>1279</v>
       </c>
       <c r="O859" s="1" t="s">
-        <v>1280</v>
+        <v>1279</v>
       </c>
       <c r="P859" s="1" t="s">
-        <v>1280</v>
+        <v>1279</v>
       </c>
       <c r="Q859" s="1" t="s">
-        <v>1280</v>
+        <v>1279</v>
       </c>
       <c r="S859" s="1" t="s">
-        <v>1280</v>
+        <v>1279</v>
       </c>
       <c r="X859" s="1" t="s">
         <v>175</v>
@@ -53427,28 +53424,28 @@
     </row>
     <row r="860" spans="1:24" ht="15">
       <c r="A860" s="1" t="s">
-        <v>1241</v>
+        <v>1240</v>
       </c>
       <c r="D860" s="1" t="s">
-        <v>1278</v>
+        <v>1277</v>
       </c>
       <c r="E860" s="17">
         <v>43124</v>
       </c>
       <c r="F860" s="1" t="s">
-        <v>1281</v>
+        <v>1280</v>
       </c>
       <c r="G860" s="1" t="s">
-        <v>1284</v>
+        <v>1283</v>
       </c>
       <c r="H860" s="1" t="s">
-        <v>1284</v>
+        <v>1283</v>
       </c>
       <c r="I860" s="1" t="s">
         <v>169</v>
       </c>
       <c r="J860" s="1" t="s">
-        <v>1280</v>
+        <v>1279</v>
       </c>
       <c r="K860" s="9" t="s">
         <v>170</v>
@@ -53457,19 +53454,19 @@
         <v>954</v>
       </c>
       <c r="N860" s="1" t="s">
-        <v>1280</v>
+        <v>1279</v>
       </c>
       <c r="O860" s="1" t="s">
-        <v>1280</v>
+        <v>1279</v>
       </c>
       <c r="P860" s="1" t="s">
-        <v>1280</v>
+        <v>1279</v>
       </c>
       <c r="Q860" s="1" t="s">
-        <v>1280</v>
+        <v>1279</v>
       </c>
       <c r="S860" s="1" t="s">
-        <v>1280</v>
+        <v>1279</v>
       </c>
       <c r="X860" s="1" t="s">
         <v>175</v>
@@ -53477,28 +53474,28 @@
     </row>
     <row r="861" spans="1:24" ht="15">
       <c r="A861" s="1" t="s">
-        <v>1242</v>
+        <v>1241</v>
       </c>
       <c r="D861" s="1" t="s">
-        <v>1278</v>
+        <v>1277</v>
       </c>
       <c r="E861" s="17">
         <v>43124</v>
       </c>
       <c r="F861" s="1" t="s">
-        <v>1281</v>
+        <v>1280</v>
       </c>
       <c r="G861" s="1" t="s">
-        <v>1283</v>
+        <v>1282</v>
       </c>
       <c r="H861" s="1" t="s">
-        <v>1283</v>
+        <v>1282</v>
       </c>
       <c r="I861" s="1" t="s">
         <v>169</v>
       </c>
       <c r="J861" s="1" t="s">
-        <v>1280</v>
+        <v>1279</v>
       </c>
       <c r="K861" s="9" t="s">
         <v>170</v>
@@ -53507,19 +53504,19 @@
         <v>954</v>
       </c>
       <c r="N861" s="1" t="s">
-        <v>1280</v>
+        <v>1279</v>
       </c>
       <c r="O861" s="1" t="s">
-        <v>1280</v>
+        <v>1279</v>
       </c>
       <c r="P861" s="1" t="s">
-        <v>1280</v>
+        <v>1279</v>
       </c>
       <c r="Q861" s="1" t="s">
-        <v>1280</v>
+        <v>1279</v>
       </c>
       <c r="S861" s="1" t="s">
-        <v>1280</v>
+        <v>1279</v>
       </c>
       <c r="X861" s="1" t="s">
         <v>175</v>
@@ -53527,28 +53524,28 @@
     </row>
     <row r="862" spans="1:24" ht="15">
       <c r="A862" s="1" t="s">
-        <v>1255</v>
+        <v>1254</v>
       </c>
       <c r="D862" s="1" t="s">
-        <v>1278</v>
+        <v>1277</v>
       </c>
       <c r="E862" s="17">
         <v>43124</v>
       </c>
       <c r="F862" s="1" t="s">
-        <v>1281</v>
+        <v>1280</v>
       </c>
       <c r="G862" s="1" t="s">
-        <v>1284</v>
+        <v>1283</v>
       </c>
       <c r="H862" s="1" t="s">
-        <v>1284</v>
+        <v>1283</v>
       </c>
       <c r="I862" s="1" t="s">
         <v>169</v>
       </c>
       <c r="J862" s="1" t="s">
-        <v>1280</v>
+        <v>1279</v>
       </c>
       <c r="K862" s="9" t="s">
         <v>170</v>
@@ -53557,19 +53554,19 @@
         <v>954</v>
       </c>
       <c r="N862" s="1" t="s">
-        <v>1280</v>
+        <v>1279</v>
       </c>
       <c r="O862" s="1" t="s">
-        <v>1280</v>
+        <v>1279</v>
       </c>
       <c r="P862" s="1" t="s">
-        <v>1280</v>
+        <v>1279</v>
       </c>
       <c r="Q862" s="1" t="s">
-        <v>1280</v>
+        <v>1279</v>
       </c>
       <c r="S862" s="1" t="s">
-        <v>1280</v>
+        <v>1279</v>
       </c>
       <c r="X862" s="1" t="s">
         <v>175</v>
@@ -53577,28 +53574,28 @@
     </row>
     <row r="863" spans="1:24" ht="15">
       <c r="A863" s="1" t="s">
-        <v>1243</v>
+        <v>1242</v>
       </c>
       <c r="D863" s="1" t="s">
-        <v>1278</v>
+        <v>1277</v>
       </c>
       <c r="E863" s="17">
         <v>43124</v>
       </c>
       <c r="F863" s="1" t="s">
-        <v>1281</v>
+        <v>1280</v>
       </c>
       <c r="G863" s="1" t="s">
-        <v>1283</v>
+        <v>1282</v>
       </c>
       <c r="H863" s="1" t="s">
-        <v>1283</v>
+        <v>1282</v>
       </c>
       <c r="I863" s="1" t="s">
         <v>169</v>
       </c>
       <c r="J863" s="1" t="s">
-        <v>1280</v>
+        <v>1279</v>
       </c>
       <c r="K863" s="9" t="s">
         <v>170</v>
@@ -53607,19 +53604,19 @@
         <v>954</v>
       </c>
       <c r="N863" s="1" t="s">
-        <v>1280</v>
+        <v>1279</v>
       </c>
       <c r="O863" s="1" t="s">
-        <v>1280</v>
+        <v>1279</v>
       </c>
       <c r="P863" s="1" t="s">
-        <v>1280</v>
+        <v>1279</v>
       </c>
       <c r="Q863" s="1" t="s">
-        <v>1280</v>
+        <v>1279</v>
       </c>
       <c r="S863" s="1" t="s">
-        <v>1280</v>
+        <v>1279</v>
       </c>
       <c r="X863" s="1" t="s">
         <v>175</v>
@@ -53627,28 +53624,28 @@
     </row>
     <row r="864" spans="1:24" ht="15">
       <c r="A864" s="1" t="s">
-        <v>1244</v>
+        <v>1243</v>
       </c>
       <c r="D864" s="1" t="s">
-        <v>1278</v>
+        <v>1277</v>
       </c>
       <c r="E864" s="17">
         <v>43124</v>
       </c>
       <c r="F864" s="1" t="s">
-        <v>1281</v>
+        <v>1280</v>
       </c>
       <c r="G864" s="1" t="s">
-        <v>1283</v>
+        <v>1282</v>
       </c>
       <c r="H864" s="1" t="s">
-        <v>1283</v>
+        <v>1282</v>
       </c>
       <c r="I864" s="1" t="s">
         <v>169</v>
       </c>
       <c r="J864" s="1" t="s">
-        <v>1280</v>
+        <v>1279</v>
       </c>
       <c r="K864" s="9" t="s">
         <v>170</v>
@@ -53657,19 +53654,19 @@
         <v>954</v>
       </c>
       <c r="N864" s="1" t="s">
-        <v>1280</v>
+        <v>1279</v>
       </c>
       <c r="O864" s="1" t="s">
-        <v>1280</v>
+        <v>1279</v>
       </c>
       <c r="P864" s="1" t="s">
-        <v>1280</v>
+        <v>1279</v>
       </c>
       <c r="Q864" s="1" t="s">
-        <v>1280</v>
+        <v>1279</v>
       </c>
       <c r="S864" s="1" t="s">
-        <v>1280</v>
+        <v>1279</v>
       </c>
       <c r="X864" s="1" t="s">
         <v>175</v>
@@ -53677,28 +53674,28 @@
     </row>
     <row r="865" spans="1:24" ht="15">
       <c r="A865" s="1" t="s">
-        <v>1245</v>
+        <v>1244</v>
       </c>
       <c r="D865" s="1" t="s">
-        <v>1278</v>
+        <v>1277</v>
       </c>
       <c r="E865" s="17">
         <v>43124</v>
       </c>
       <c r="F865" s="1" t="s">
-        <v>1281</v>
+        <v>1280</v>
       </c>
       <c r="G865" s="1" t="s">
-        <v>1284</v>
+        <v>1283</v>
       </c>
       <c r="H865" s="1" t="s">
-        <v>1284</v>
+        <v>1283</v>
       </c>
       <c r="I865" s="1" t="s">
         <v>169</v>
       </c>
       <c r="J865" s="1" t="s">
-        <v>1280</v>
+        <v>1279</v>
       </c>
       <c r="K865" s="9" t="s">
         <v>170</v>
@@ -53707,19 +53704,19 @@
         <v>954</v>
       </c>
       <c r="N865" s="1" t="s">
-        <v>1280</v>
+        <v>1279</v>
       </c>
       <c r="O865" s="1" t="s">
-        <v>1280</v>
+        <v>1279</v>
       </c>
       <c r="P865" s="1" t="s">
-        <v>1280</v>
+        <v>1279</v>
       </c>
       <c r="Q865" s="1" t="s">
-        <v>1280</v>
+        <v>1279</v>
       </c>
       <c r="S865" s="1" t="s">
-        <v>1280</v>
+        <v>1279</v>
       </c>
       <c r="X865" s="1" t="s">
         <v>175</v>
@@ -53727,28 +53724,28 @@
     </row>
     <row r="866" spans="1:24" ht="15">
       <c r="A866" s="1" t="s">
-        <v>1246</v>
+        <v>1245</v>
       </c>
       <c r="D866" s="1" t="s">
-        <v>1278</v>
+        <v>1277</v>
       </c>
       <c r="E866" s="17">
         <v>43124</v>
       </c>
       <c r="F866" s="1" t="s">
-        <v>1281</v>
+        <v>1280</v>
       </c>
       <c r="G866" s="1" t="s">
-        <v>1284</v>
+        <v>1283</v>
       </c>
       <c r="H866" s="1" t="s">
-        <v>1284</v>
+        <v>1283</v>
       </c>
       <c r="I866" s="1" t="s">
         <v>169</v>
       </c>
       <c r="J866" s="1" t="s">
-        <v>1280</v>
+        <v>1279</v>
       </c>
       <c r="K866" s="9" t="s">
         <v>170</v>
@@ -53757,19 +53754,19 @@
         <v>954</v>
       </c>
       <c r="N866" s="1" t="s">
-        <v>1280</v>
+        <v>1279</v>
       </c>
       <c r="O866" s="1" t="s">
-        <v>1280</v>
+        <v>1279</v>
       </c>
       <c r="P866" s="1" t="s">
-        <v>1280</v>
+        <v>1279</v>
       </c>
       <c r="Q866" s="1" t="s">
-        <v>1280</v>
+        <v>1279</v>
       </c>
       <c r="S866" s="1" t="s">
-        <v>1280</v>
+        <v>1279</v>
       </c>
       <c r="X866" s="1" t="s">
         <v>175</v>
@@ -53777,28 +53774,28 @@
     </row>
     <row r="867" spans="1:24" ht="15">
       <c r="A867" s="1" t="s">
-        <v>1247</v>
+        <v>1246</v>
       </c>
       <c r="D867" s="1" t="s">
-        <v>1278</v>
+        <v>1277</v>
       </c>
       <c r="E867" s="17">
         <v>43124</v>
       </c>
       <c r="F867" s="1" t="s">
-        <v>1281</v>
+        <v>1280</v>
       </c>
       <c r="G867" s="1" t="s">
-        <v>1283</v>
+        <v>1282</v>
       </c>
       <c r="H867" s="1" t="s">
-        <v>1283</v>
+        <v>1282</v>
       </c>
       <c r="I867" s="1" t="s">
         <v>169</v>
       </c>
       <c r="J867" s="1" t="s">
-        <v>1280</v>
+        <v>1279</v>
       </c>
       <c r="K867" s="9" t="s">
         <v>170</v>
@@ -53807,19 +53804,19 @@
         <v>954</v>
       </c>
       <c r="N867" s="1" t="s">
-        <v>1280</v>
+        <v>1279</v>
       </c>
       <c r="O867" s="1" t="s">
-        <v>1280</v>
+        <v>1279</v>
       </c>
       <c r="P867" s="1" t="s">
-        <v>1280</v>
+        <v>1279</v>
       </c>
       <c r="Q867" s="1" t="s">
-        <v>1280</v>
+        <v>1279</v>
       </c>
       <c r="S867" s="1" t="s">
-        <v>1280</v>
+        <v>1279</v>
       </c>
       <c r="X867" s="1" t="s">
         <v>175</v>
@@ -53827,28 +53824,28 @@
     </row>
     <row r="868" spans="1:24" ht="15">
       <c r="A868" s="1" t="s">
-        <v>1248</v>
+        <v>1247</v>
       </c>
       <c r="D868" s="1" t="s">
-        <v>1278</v>
+        <v>1277</v>
       </c>
       <c r="E868" s="17">
         <v>43124</v>
       </c>
       <c r="F868" s="1" t="s">
-        <v>1281</v>
+        <v>1280</v>
       </c>
       <c r="G868" s="1" t="s">
-        <v>1284</v>
+        <v>1283</v>
       </c>
       <c r="H868" s="1" t="s">
-        <v>1284</v>
+        <v>1283</v>
       </c>
       <c r="I868" s="1" t="s">
         <v>169</v>
       </c>
       <c r="J868" s="1" t="s">
-        <v>1280</v>
+        <v>1279</v>
       </c>
       <c r="K868" s="9" t="s">
         <v>170</v>
@@ -53857,19 +53854,19 @@
         <v>954</v>
       </c>
       <c r="N868" s="1" t="s">
-        <v>1280</v>
+        <v>1279</v>
       </c>
       <c r="O868" s="1" t="s">
-        <v>1280</v>
+        <v>1279</v>
       </c>
       <c r="P868" s="1" t="s">
-        <v>1280</v>
+        <v>1279</v>
       </c>
       <c r="Q868" s="1" t="s">
-        <v>1280</v>
+        <v>1279</v>
       </c>
       <c r="S868" s="1" t="s">
-        <v>1280</v>
+        <v>1279</v>
       </c>
       <c r="X868" s="1" t="s">
         <v>175</v>
@@ -53877,28 +53874,28 @@
     </row>
     <row r="869" spans="1:24" ht="15">
       <c r="A869" s="1" t="s">
-        <v>1249</v>
+        <v>1248</v>
       </c>
       <c r="D869" s="1" t="s">
-        <v>1278</v>
+        <v>1277</v>
       </c>
       <c r="E869" s="17">
         <v>43124</v>
       </c>
       <c r="F869" s="1" t="s">
-        <v>1281</v>
+        <v>1280</v>
       </c>
       <c r="G869" s="1" t="s">
-        <v>1283</v>
+        <v>1282</v>
       </c>
       <c r="H869" s="1" t="s">
-        <v>1283</v>
+        <v>1282</v>
       </c>
       <c r="I869" s="1" t="s">
         <v>169</v>
       </c>
       <c r="J869" s="1" t="s">
-        <v>1280</v>
+        <v>1279</v>
       </c>
       <c r="K869" s="9" t="s">
         <v>170</v>
@@ -53907,19 +53904,19 @@
         <v>954</v>
       </c>
       <c r="N869" s="1" t="s">
-        <v>1280</v>
+        <v>1279</v>
       </c>
       <c r="O869" s="1" t="s">
-        <v>1280</v>
+        <v>1279</v>
       </c>
       <c r="P869" s="1" t="s">
-        <v>1280</v>
+        <v>1279</v>
       </c>
       <c r="Q869" s="1" t="s">
-        <v>1280</v>
+        <v>1279</v>
       </c>
       <c r="S869" s="1" t="s">
-        <v>1280</v>
+        <v>1279</v>
       </c>
       <c r="X869" s="1" t="s">
         <v>175</v>
@@ -53927,28 +53924,28 @@
     </row>
     <row r="870" spans="1:24" ht="15">
       <c r="A870" s="1" t="s">
-        <v>1250</v>
+        <v>1249</v>
       </c>
       <c r="D870" s="1" t="s">
-        <v>1278</v>
+        <v>1277</v>
       </c>
       <c r="E870" s="17">
         <v>43124</v>
       </c>
       <c r="F870" s="1" t="s">
-        <v>1281</v>
+        <v>1280</v>
       </c>
       <c r="G870" s="1" t="s">
-        <v>1284</v>
+        <v>1283</v>
       </c>
       <c r="H870" s="1" t="s">
-        <v>1284</v>
+        <v>1283</v>
       </c>
       <c r="I870" s="1" t="s">
         <v>169</v>
       </c>
       <c r="J870" s="1" t="s">
-        <v>1280</v>
+        <v>1279</v>
       </c>
       <c r="K870" s="9" t="s">
         <v>170</v>
@@ -53957,19 +53954,19 @@
         <v>954</v>
       </c>
       <c r="N870" s="1" t="s">
-        <v>1280</v>
+        <v>1279</v>
       </c>
       <c r="O870" s="1" t="s">
-        <v>1280</v>
+        <v>1279</v>
       </c>
       <c r="P870" s="1" t="s">
-        <v>1280</v>
+        <v>1279</v>
       </c>
       <c r="Q870" s="1" t="s">
-        <v>1280</v>
+        <v>1279</v>
       </c>
       <c r="S870" s="1" t="s">
-        <v>1280</v>
+        <v>1279</v>
       </c>
       <c r="X870" s="1" t="s">
         <v>175</v>
@@ -53977,28 +53974,28 @@
     </row>
     <row r="871" spans="1:24" ht="15">
       <c r="A871" s="1" t="s">
-        <v>1251</v>
+        <v>1250</v>
       </c>
       <c r="D871" s="1" t="s">
-        <v>1278</v>
+        <v>1277</v>
       </c>
       <c r="E871" s="17">
         <v>43124</v>
       </c>
       <c r="F871" s="1" t="s">
-        <v>1281</v>
+        <v>1280</v>
       </c>
       <c r="G871" s="1" t="s">
-        <v>1283</v>
+        <v>1282</v>
       </c>
       <c r="H871" s="1" t="s">
-        <v>1283</v>
+        <v>1282</v>
       </c>
       <c r="I871" s="1" t="s">
         <v>169</v>
       </c>
       <c r="J871" s="1" t="s">
-        <v>1280</v>
+        <v>1279</v>
       </c>
       <c r="K871" s="9" t="s">
         <v>170</v>
@@ -54007,19 +54004,19 @@
         <v>954</v>
       </c>
       <c r="N871" s="1" t="s">
-        <v>1280</v>
+        <v>1279</v>
       </c>
       <c r="O871" s="1" t="s">
-        <v>1280</v>
+        <v>1279</v>
       </c>
       <c r="P871" s="1" t="s">
-        <v>1280</v>
+        <v>1279</v>
       </c>
       <c r="Q871" s="1" t="s">
-        <v>1280</v>
+        <v>1279</v>
       </c>
       <c r="S871" s="1" t="s">
-        <v>1280</v>
+        <v>1279</v>
       </c>
       <c r="X871" s="1" t="s">
         <v>175</v>
@@ -54027,28 +54024,28 @@
     </row>
     <row r="872" spans="1:24" ht="15">
       <c r="A872" s="23" t="s">
-        <v>1252</v>
+        <v>1251</v>
       </c>
       <c r="D872" s="1" t="s">
-        <v>1278</v>
+        <v>1277</v>
       </c>
       <c r="E872" s="17">
         <v>43124</v>
       </c>
       <c r="F872" s="1" t="s">
-        <v>1281</v>
+        <v>1280</v>
       </c>
       <c r="G872" s="1" t="s">
-        <v>1284</v>
+        <v>1283</v>
       </c>
       <c r="H872" s="1" t="s">
-        <v>1284</v>
+        <v>1283</v>
       </c>
       <c r="I872" s="1" t="s">
         <v>169</v>
       </c>
       <c r="J872" s="1" t="s">
-        <v>1280</v>
+        <v>1279</v>
       </c>
       <c r="K872" s="9" t="s">
         <v>170</v>
@@ -54057,19 +54054,19 @@
         <v>954</v>
       </c>
       <c r="N872" s="1" t="s">
-        <v>1280</v>
+        <v>1279</v>
       </c>
       <c r="O872" s="1" t="s">
-        <v>1280</v>
+        <v>1279</v>
       </c>
       <c r="P872" s="1" t="s">
-        <v>1280</v>
+        <v>1279</v>
       </c>
       <c r="Q872" s="1" t="s">
-        <v>1280</v>
+        <v>1279</v>
       </c>
       <c r="S872" s="1" t="s">
-        <v>1280</v>
+        <v>1279</v>
       </c>
       <c r="X872" s="1" t="s">
         <v>175</v>
@@ -54077,28 +54074,28 @@
     </row>
     <row r="873" spans="1:24" ht="15">
       <c r="A873" s="23" t="s">
-        <v>1253</v>
+        <v>1252</v>
       </c>
       <c r="D873" s="1" t="s">
-        <v>1278</v>
+        <v>1277</v>
       </c>
       <c r="E873" s="17">
         <v>43124</v>
       </c>
       <c r="F873" s="1" t="s">
-        <v>1281</v>
+        <v>1280</v>
       </c>
       <c r="G873" s="1" t="s">
-        <v>1283</v>
+        <v>1282</v>
       </c>
       <c r="H873" s="1" t="s">
-        <v>1283</v>
+        <v>1282</v>
       </c>
       <c r="I873" s="1" t="s">
         <v>169</v>
       </c>
       <c r="J873" s="1" t="s">
-        <v>1280</v>
+        <v>1279</v>
       </c>
       <c r="K873" s="9" t="s">
         <v>170</v>
@@ -54107,19 +54104,19 @@
         <v>954</v>
       </c>
       <c r="N873" s="1" t="s">
-        <v>1280</v>
+        <v>1279</v>
       </c>
       <c r="O873" s="1" t="s">
-        <v>1280</v>
+        <v>1279</v>
       </c>
       <c r="P873" s="1" t="s">
-        <v>1280</v>
+        <v>1279</v>
       </c>
       <c r="Q873" s="1" t="s">
-        <v>1280</v>
+        <v>1279</v>
       </c>
       <c r="S873" s="1" t="s">
-        <v>1280</v>
+        <v>1279</v>
       </c>
       <c r="X873" s="1" t="s">
         <v>175</v>
@@ -54127,895 +54124,895 @@
     </row>
     <row r="874" spans="1:24">
       <c r="A874" s="1" t="s">
-        <v>1256</v>
+        <v>1255</v>
       </c>
       <c r="D874" s="1" t="s">
+        <v>1278</v>
+      </c>
+      <c r="F874" s="1" t="s">
+        <v>1280</v>
+      </c>
+      <c r="G874" s="1" t="s">
+        <v>1284</v>
+      </c>
+      <c r="H874" s="1" t="s">
+        <v>1284</v>
+      </c>
+      <c r="I874" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="J874" s="1" t="s">
         <v>1279</v>
       </c>
-      <c r="F874" s="1" t="s">
-        <v>1281</v>
-      </c>
-      <c r="G874" s="1" t="s">
+      <c r="K874" s="9" t="s">
         <v>1285</v>
-      </c>
-      <c r="H874" s="1" t="s">
-        <v>1285</v>
-      </c>
-      <c r="I874" s="1" t="s">
-        <v>169</v>
-      </c>
-      <c r="J874" s="1" t="s">
-        <v>1280</v>
-      </c>
-      <c r="K874" s="9" t="s">
-        <v>1286</v>
       </c>
       <c r="M874" s="1" t="s">
         <v>954</v>
       </c>
       <c r="N874" s="1" t="s">
-        <v>1280</v>
+        <v>1279</v>
       </c>
       <c r="O874" s="1" t="s">
-        <v>1280</v>
+        <v>1279</v>
       </c>
       <c r="P874" s="1" t="s">
-        <v>1280</v>
+        <v>1279</v>
       </c>
       <c r="Q874" s="1" t="s">
-        <v>1280</v>
+        <v>1279</v>
       </c>
       <c r="S874" s="1" t="s">
-        <v>1280</v>
+        <v>1279</v>
       </c>
       <c r="X874" s="1" t="s">
-        <v>1280</v>
+        <v>1279</v>
       </c>
     </row>
     <row r="875" spans="1:24">
       <c r="A875" s="1" t="s">
-        <v>1257</v>
+        <v>1256</v>
       </c>
       <c r="D875" s="1" t="s">
+        <v>1278</v>
+      </c>
+      <c r="F875" s="1" t="s">
+        <v>1280</v>
+      </c>
+      <c r="G875" s="1" t="s">
+        <v>1284</v>
+      </c>
+      <c r="H875" s="1" t="s">
+        <v>1284</v>
+      </c>
+      <c r="I875" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="J875" s="1" t="s">
         <v>1279</v>
       </c>
-      <c r="F875" s="1" t="s">
-        <v>1281</v>
-      </c>
-      <c r="G875" s="1" t="s">
+      <c r="K875" s="9" t="s">
         <v>1285</v>
-      </c>
-      <c r="H875" s="1" t="s">
-        <v>1285</v>
-      </c>
-      <c r="I875" s="1" t="s">
-        <v>169</v>
-      </c>
-      <c r="J875" s="1" t="s">
-        <v>1280</v>
-      </c>
-      <c r="K875" s="9" t="s">
-        <v>1286</v>
       </c>
       <c r="M875" s="1" t="s">
         <v>954</v>
       </c>
       <c r="N875" s="1" t="s">
-        <v>1280</v>
+        <v>1279</v>
       </c>
       <c r="O875" s="1" t="s">
-        <v>1280</v>
+        <v>1279</v>
       </c>
       <c r="P875" s="1" t="s">
-        <v>1280</v>
+        <v>1279</v>
       </c>
       <c r="Q875" s="1" t="s">
-        <v>1280</v>
+        <v>1279</v>
       </c>
       <c r="S875" s="1" t="s">
-        <v>1280</v>
+        <v>1279</v>
       </c>
       <c r="X875" s="1" t="s">
-        <v>1280</v>
+        <v>1279</v>
       </c>
     </row>
     <row r="876" spans="1:24">
       <c r="A876" s="1" t="s">
-        <v>1258</v>
+        <v>1257</v>
       </c>
       <c r="D876" s="1" t="s">
+        <v>1278</v>
+      </c>
+      <c r="F876" s="1" t="s">
+        <v>1280</v>
+      </c>
+      <c r="G876" s="1" t="s">
+        <v>1284</v>
+      </c>
+      <c r="H876" s="1" t="s">
+        <v>1284</v>
+      </c>
+      <c r="I876" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="J876" s="1" t="s">
         <v>1279</v>
       </c>
-      <c r="F876" s="1" t="s">
-        <v>1281</v>
-      </c>
-      <c r="G876" s="1" t="s">
+      <c r="K876" s="9" t="s">
         <v>1285</v>
-      </c>
-      <c r="H876" s="1" t="s">
-        <v>1285</v>
-      </c>
-      <c r="I876" s="1" t="s">
-        <v>169</v>
-      </c>
-      <c r="J876" s="1" t="s">
-        <v>1280</v>
-      </c>
-      <c r="K876" s="9" t="s">
-        <v>1286</v>
       </c>
       <c r="M876" s="1" t="s">
         <v>954</v>
       </c>
       <c r="N876" s="1" t="s">
-        <v>1280</v>
+        <v>1279</v>
       </c>
       <c r="O876" s="1" t="s">
-        <v>1280</v>
+        <v>1279</v>
       </c>
       <c r="P876" s="1" t="s">
-        <v>1280</v>
+        <v>1279</v>
       </c>
       <c r="Q876" s="1" t="s">
-        <v>1280</v>
+        <v>1279</v>
       </c>
       <c r="S876" s="1" t="s">
-        <v>1280</v>
+        <v>1279</v>
       </c>
       <c r="X876" s="1" t="s">
-        <v>1280</v>
+        <v>1279</v>
       </c>
     </row>
     <row r="877" spans="1:24">
       <c r="A877" s="1" t="s">
-        <v>1259</v>
+        <v>1258</v>
       </c>
       <c r="D877" s="1" t="s">
+        <v>1278</v>
+      </c>
+      <c r="F877" s="1" t="s">
+        <v>1280</v>
+      </c>
+      <c r="G877" s="1" t="s">
+        <v>1284</v>
+      </c>
+      <c r="H877" s="1" t="s">
+        <v>1284</v>
+      </c>
+      <c r="I877" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="J877" s="1" t="s">
         <v>1279</v>
       </c>
-      <c r="F877" s="1" t="s">
-        <v>1281</v>
-      </c>
-      <c r="G877" s="1" t="s">
+      <c r="K877" s="9" t="s">
         <v>1285</v>
-      </c>
-      <c r="H877" s="1" t="s">
-        <v>1285</v>
-      </c>
-      <c r="I877" s="1" t="s">
-        <v>169</v>
-      </c>
-      <c r="J877" s="1" t="s">
-        <v>1280</v>
-      </c>
-      <c r="K877" s="9" t="s">
-        <v>1286</v>
       </c>
       <c r="M877" s="1" t="s">
         <v>954</v>
       </c>
       <c r="N877" s="1" t="s">
-        <v>1280</v>
+        <v>1279</v>
       </c>
       <c r="O877" s="1" t="s">
-        <v>1280</v>
+        <v>1279</v>
       </c>
       <c r="P877" s="1" t="s">
-        <v>1280</v>
+        <v>1279</v>
       </c>
       <c r="Q877" s="1" t="s">
-        <v>1280</v>
+        <v>1279</v>
       </c>
       <c r="S877" s="1" t="s">
-        <v>1280</v>
+        <v>1279</v>
       </c>
       <c r="X877" s="1" t="s">
-        <v>1280</v>
+        <v>1279</v>
       </c>
     </row>
     <row r="878" spans="1:24">
       <c r="A878" s="23" t="s">
-        <v>1260</v>
+        <v>1259</v>
       </c>
       <c r="D878" s="1" t="s">
+        <v>1278</v>
+      </c>
+      <c r="F878" s="1" t="s">
+        <v>1280</v>
+      </c>
+      <c r="G878" s="1" t="s">
+        <v>1284</v>
+      </c>
+      <c r="H878" s="1" t="s">
+        <v>1284</v>
+      </c>
+      <c r="I878" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="J878" s="1" t="s">
         <v>1279</v>
       </c>
-      <c r="F878" s="1" t="s">
-        <v>1281</v>
-      </c>
-      <c r="G878" s="1" t="s">
+      <c r="K878" s="9" t="s">
         <v>1285</v>
-      </c>
-      <c r="H878" s="1" t="s">
-        <v>1285</v>
-      </c>
-      <c r="I878" s="1" t="s">
-        <v>169</v>
-      </c>
-      <c r="J878" s="1" t="s">
-        <v>1280</v>
-      </c>
-      <c r="K878" s="9" t="s">
-        <v>1286</v>
       </c>
       <c r="M878" s="1" t="s">
         <v>954</v>
       </c>
       <c r="N878" s="1" t="s">
-        <v>1280</v>
+        <v>1279</v>
       </c>
       <c r="O878" s="1" t="s">
-        <v>1280</v>
+        <v>1279</v>
       </c>
       <c r="P878" s="1" t="s">
-        <v>1280</v>
+        <v>1279</v>
       </c>
       <c r="Q878" s="1" t="s">
-        <v>1280</v>
+        <v>1279</v>
       </c>
       <c r="S878" s="1" t="s">
-        <v>1280</v>
+        <v>1279</v>
       </c>
       <c r="X878" s="1" t="s">
-        <v>1280</v>
+        <v>1279</v>
       </c>
     </row>
     <row r="879" spans="1:24">
       <c r="A879" s="23" t="s">
-        <v>1261</v>
+        <v>1260</v>
       </c>
       <c r="D879" s="1" t="s">
+        <v>1278</v>
+      </c>
+      <c r="F879" s="1" t="s">
+        <v>1280</v>
+      </c>
+      <c r="G879" s="1" t="s">
+        <v>1284</v>
+      </c>
+      <c r="H879" s="1" t="s">
+        <v>1284</v>
+      </c>
+      <c r="I879" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="J879" s="1" t="s">
         <v>1279</v>
       </c>
-      <c r="F879" s="1" t="s">
-        <v>1281</v>
-      </c>
-      <c r="G879" s="1" t="s">
+      <c r="K879" s="9" t="s">
         <v>1285</v>
-      </c>
-      <c r="H879" s="1" t="s">
-        <v>1285</v>
-      </c>
-      <c r="I879" s="1" t="s">
-        <v>169</v>
-      </c>
-      <c r="J879" s="1" t="s">
-        <v>1280</v>
-      </c>
-      <c r="K879" s="9" t="s">
-        <v>1286</v>
       </c>
       <c r="M879" s="1" t="s">
         <v>954</v>
       </c>
       <c r="N879" s="1" t="s">
-        <v>1280</v>
+        <v>1279</v>
       </c>
       <c r="O879" s="1" t="s">
-        <v>1280</v>
+        <v>1279</v>
       </c>
       <c r="P879" s="1" t="s">
-        <v>1280</v>
+        <v>1279</v>
       </c>
       <c r="Q879" s="1" t="s">
-        <v>1280</v>
+        <v>1279</v>
       </c>
       <c r="S879" s="1" t="s">
-        <v>1280</v>
+        <v>1279</v>
       </c>
       <c r="X879" s="1" t="s">
-        <v>1280</v>
+        <v>1279</v>
       </c>
     </row>
     <row r="880" spans="1:24">
       <c r="A880" s="23" t="s">
-        <v>1262</v>
+        <v>1261</v>
       </c>
       <c r="D880" s="1" t="s">
+        <v>1278</v>
+      </c>
+      <c r="F880" s="1" t="s">
+        <v>1280</v>
+      </c>
+      <c r="G880" s="1" t="s">
+        <v>1284</v>
+      </c>
+      <c r="H880" s="1" t="s">
+        <v>1284</v>
+      </c>
+      <c r="I880" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="J880" s="1" t="s">
         <v>1279</v>
       </c>
-      <c r="F880" s="1" t="s">
-        <v>1281</v>
-      </c>
-      <c r="G880" s="1" t="s">
+      <c r="K880" s="9" t="s">
         <v>1285</v>
-      </c>
-      <c r="H880" s="1" t="s">
-        <v>1285</v>
-      </c>
-      <c r="I880" s="1" t="s">
-        <v>169</v>
-      </c>
-      <c r="J880" s="1" t="s">
-        <v>1280</v>
-      </c>
-      <c r="K880" s="9" t="s">
-        <v>1286</v>
       </c>
       <c r="M880" s="1" t="s">
         <v>954</v>
       </c>
       <c r="N880" s="1" t="s">
-        <v>1280</v>
+        <v>1279</v>
       </c>
       <c r="O880" s="1" t="s">
-        <v>1280</v>
+        <v>1279</v>
       </c>
       <c r="P880" s="1" t="s">
-        <v>1280</v>
+        <v>1279</v>
       </c>
       <c r="Q880" s="1" t="s">
-        <v>1280</v>
+        <v>1279</v>
       </c>
       <c r="S880" s="1" t="s">
-        <v>1280</v>
+        <v>1279</v>
       </c>
       <c r="X880" s="1" t="s">
-        <v>1280</v>
+        <v>1279</v>
       </c>
     </row>
     <row r="881" spans="1:24">
       <c r="A881" s="23" t="s">
-        <v>1263</v>
+        <v>1262</v>
       </c>
       <c r="D881" s="1" t="s">
+        <v>1278</v>
+      </c>
+      <c r="F881" s="1" t="s">
+        <v>1280</v>
+      </c>
+      <c r="G881" s="1" t="s">
+        <v>1284</v>
+      </c>
+      <c r="H881" s="1" t="s">
+        <v>1284</v>
+      </c>
+      <c r="I881" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="J881" s="1" t="s">
         <v>1279</v>
       </c>
-      <c r="F881" s="1" t="s">
-        <v>1281</v>
-      </c>
-      <c r="G881" s="1" t="s">
+      <c r="K881" s="9" t="s">
         <v>1285</v>
-      </c>
-      <c r="H881" s="1" t="s">
-        <v>1285</v>
-      </c>
-      <c r="I881" s="1" t="s">
-        <v>169</v>
-      </c>
-      <c r="J881" s="1" t="s">
-        <v>1280</v>
-      </c>
-      <c r="K881" s="9" t="s">
-        <v>1286</v>
       </c>
       <c r="M881" s="1" t="s">
         <v>954</v>
       </c>
       <c r="N881" s="1" t="s">
-        <v>1280</v>
+        <v>1279</v>
       </c>
       <c r="O881" s="1" t="s">
-        <v>1280</v>
+        <v>1279</v>
       </c>
       <c r="P881" s="1" t="s">
-        <v>1280</v>
+        <v>1279</v>
       </c>
       <c r="Q881" s="1" t="s">
-        <v>1280</v>
+        <v>1279</v>
       </c>
       <c r="S881" s="1" t="s">
-        <v>1280</v>
+        <v>1279</v>
       </c>
       <c r="X881" s="1" t="s">
-        <v>1280</v>
+        <v>1279</v>
       </c>
     </row>
     <row r="882" spans="1:24">
       <c r="A882" s="23" t="s">
-        <v>1264</v>
+        <v>1263</v>
       </c>
       <c r="D882" s="1" t="s">
+        <v>1278</v>
+      </c>
+      <c r="F882" s="1" t="s">
+        <v>1280</v>
+      </c>
+      <c r="G882" s="1" t="s">
+        <v>1284</v>
+      </c>
+      <c r="H882" s="1" t="s">
+        <v>1284</v>
+      </c>
+      <c r="I882" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="J882" s="1" t="s">
         <v>1279</v>
       </c>
-      <c r="F882" s="1" t="s">
-        <v>1281</v>
-      </c>
-      <c r="G882" s="1" t="s">
+      <c r="K882" s="9" t="s">
         <v>1285</v>
-      </c>
-      <c r="H882" s="1" t="s">
-        <v>1285</v>
-      </c>
-      <c r="I882" s="1" t="s">
-        <v>169</v>
-      </c>
-      <c r="J882" s="1" t="s">
-        <v>1280</v>
-      </c>
-      <c r="K882" s="9" t="s">
-        <v>1286</v>
       </c>
       <c r="M882" s="1" t="s">
         <v>954</v>
       </c>
       <c r="N882" s="1" t="s">
-        <v>1280</v>
+        <v>1279</v>
       </c>
       <c r="O882" s="1" t="s">
-        <v>1280</v>
+        <v>1279</v>
       </c>
       <c r="P882" s="1" t="s">
-        <v>1280</v>
+        <v>1279</v>
       </c>
       <c r="Q882" s="1" t="s">
-        <v>1280</v>
+        <v>1279</v>
       </c>
       <c r="S882" s="1" t="s">
-        <v>1280</v>
+        <v>1279</v>
       </c>
       <c r="X882" s="1" t="s">
-        <v>1280</v>
+        <v>1279</v>
       </c>
     </row>
     <row r="883" spans="1:24">
       <c r="A883" s="23" t="s">
-        <v>1265</v>
+        <v>1264</v>
       </c>
       <c r="D883" s="1" t="s">
+        <v>1278</v>
+      </c>
+      <c r="F883" s="1" t="s">
+        <v>1280</v>
+      </c>
+      <c r="G883" s="1" t="s">
+        <v>1284</v>
+      </c>
+      <c r="H883" s="1" t="s">
+        <v>1284</v>
+      </c>
+      <c r="I883" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="J883" s="1" t="s">
         <v>1279</v>
       </c>
-      <c r="F883" s="1" t="s">
-        <v>1281</v>
-      </c>
-      <c r="G883" s="1" t="s">
+      <c r="K883" s="9" t="s">
         <v>1285</v>
-      </c>
-      <c r="H883" s="1" t="s">
-        <v>1285</v>
-      </c>
-      <c r="I883" s="1" t="s">
-        <v>169</v>
-      </c>
-      <c r="J883" s="1" t="s">
-        <v>1280</v>
-      </c>
-      <c r="K883" s="9" t="s">
-        <v>1286</v>
       </c>
       <c r="M883" s="1" t="s">
         <v>954</v>
       </c>
       <c r="N883" s="1" t="s">
-        <v>1280</v>
+        <v>1279</v>
       </c>
       <c r="O883" s="1" t="s">
-        <v>1280</v>
+        <v>1279</v>
       </c>
       <c r="P883" s="1" t="s">
-        <v>1280</v>
+        <v>1279</v>
       </c>
       <c r="Q883" s="1" t="s">
-        <v>1280</v>
+        <v>1279</v>
       </c>
       <c r="S883" s="1" t="s">
-        <v>1280</v>
+        <v>1279</v>
       </c>
       <c r="X883" s="1" t="s">
-        <v>1280</v>
+        <v>1279</v>
       </c>
     </row>
     <row r="884" spans="1:24">
       <c r="A884" s="23" t="s">
-        <v>1266</v>
+        <v>1265</v>
       </c>
       <c r="D884" s="1" t="s">
+        <v>1278</v>
+      </c>
+      <c r="F884" s="1" t="s">
+        <v>1280</v>
+      </c>
+      <c r="G884" s="1" t="s">
+        <v>1284</v>
+      </c>
+      <c r="H884" s="1" t="s">
+        <v>1284</v>
+      </c>
+      <c r="I884" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="J884" s="1" t="s">
         <v>1279</v>
       </c>
-      <c r="F884" s="1" t="s">
-        <v>1281</v>
-      </c>
-      <c r="G884" s="1" t="s">
+      <c r="K884" s="9" t="s">
         <v>1285</v>
-      </c>
-      <c r="H884" s="1" t="s">
-        <v>1285</v>
-      </c>
-      <c r="I884" s="1" t="s">
-        <v>169</v>
-      </c>
-      <c r="J884" s="1" t="s">
-        <v>1280</v>
-      </c>
-      <c r="K884" s="9" t="s">
-        <v>1286</v>
       </c>
       <c r="M884" s="1" t="s">
         <v>954</v>
       </c>
       <c r="N884" s="1" t="s">
-        <v>1280</v>
+        <v>1279</v>
       </c>
       <c r="O884" s="1" t="s">
-        <v>1280</v>
+        <v>1279</v>
       </c>
       <c r="P884" s="1" t="s">
-        <v>1280</v>
+        <v>1279</v>
       </c>
       <c r="Q884" s="1" t="s">
-        <v>1280</v>
+        <v>1279</v>
       </c>
       <c r="S884" s="1" t="s">
-        <v>1280</v>
+        <v>1279</v>
       </c>
       <c r="X884" s="1" t="s">
-        <v>1280</v>
+        <v>1279</v>
       </c>
     </row>
     <row r="885" spans="1:24">
       <c r="A885" s="23" t="s">
-        <v>1267</v>
+        <v>1266</v>
       </c>
       <c r="D885" s="1" t="s">
+        <v>1278</v>
+      </c>
+      <c r="F885" s="1" t="s">
+        <v>1280</v>
+      </c>
+      <c r="G885" s="1" t="s">
+        <v>1284</v>
+      </c>
+      <c r="H885" s="1" t="s">
+        <v>1284</v>
+      </c>
+      <c r="I885" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="J885" s="1" t="s">
         <v>1279</v>
       </c>
-      <c r="F885" s="1" t="s">
-        <v>1281</v>
-      </c>
-      <c r="G885" s="1" t="s">
+      <c r="K885" s="9" t="s">
         <v>1285</v>
-      </c>
-      <c r="H885" s="1" t="s">
-        <v>1285</v>
-      </c>
-      <c r="I885" s="1" t="s">
-        <v>169</v>
-      </c>
-      <c r="J885" s="1" t="s">
-        <v>1280</v>
-      </c>
-      <c r="K885" s="9" t="s">
-        <v>1286</v>
       </c>
       <c r="M885" s="1" t="s">
         <v>954</v>
       </c>
       <c r="N885" s="1" t="s">
-        <v>1280</v>
+        <v>1279</v>
       </c>
       <c r="O885" s="1" t="s">
-        <v>1280</v>
+        <v>1279</v>
       </c>
       <c r="P885" s="1" t="s">
-        <v>1280</v>
+        <v>1279</v>
       </c>
       <c r="Q885" s="1" t="s">
-        <v>1280</v>
+        <v>1279</v>
       </c>
       <c r="S885" s="1" t="s">
-        <v>1280</v>
+        <v>1279</v>
       </c>
       <c r="X885" s="1" t="s">
-        <v>1280</v>
+        <v>1279</v>
       </c>
     </row>
     <row r="886" spans="1:24">
       <c r="A886" s="23" t="s">
-        <v>1268</v>
+        <v>1267</v>
       </c>
       <c r="D886" s="1" t="s">
+        <v>1278</v>
+      </c>
+      <c r="F886" s="1" t="s">
+        <v>1280</v>
+      </c>
+      <c r="G886" s="1" t="s">
+        <v>1284</v>
+      </c>
+      <c r="H886" s="1" t="s">
+        <v>1284</v>
+      </c>
+      <c r="I886" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="J886" s="1" t="s">
         <v>1279</v>
       </c>
-      <c r="F886" s="1" t="s">
-        <v>1281</v>
-      </c>
-      <c r="G886" s="1" t="s">
+      <c r="K886" s="9" t="s">
         <v>1285</v>
-      </c>
-      <c r="H886" s="1" t="s">
-        <v>1285</v>
-      </c>
-      <c r="I886" s="1" t="s">
-        <v>169</v>
-      </c>
-      <c r="J886" s="1" t="s">
-        <v>1280</v>
-      </c>
-      <c r="K886" s="9" t="s">
-        <v>1286</v>
       </c>
       <c r="M886" s="1" t="s">
         <v>954</v>
       </c>
       <c r="N886" s="1" t="s">
-        <v>1280</v>
+        <v>1279</v>
       </c>
       <c r="O886" s="1" t="s">
-        <v>1280</v>
+        <v>1279</v>
       </c>
       <c r="P886" s="1" t="s">
-        <v>1280</v>
+        <v>1279</v>
       </c>
       <c r="Q886" s="1" t="s">
-        <v>1280</v>
+        <v>1279</v>
       </c>
       <c r="S886" s="1" t="s">
-        <v>1280</v>
+        <v>1279</v>
       </c>
       <c r="X886" s="1" t="s">
-        <v>1280</v>
+        <v>1279</v>
       </c>
     </row>
     <row r="887" spans="1:24">
       <c r="A887" s="23" t="s">
-        <v>1269</v>
+        <v>1268</v>
       </c>
       <c r="D887" s="1" t="s">
+        <v>1278</v>
+      </c>
+      <c r="F887" s="1" t="s">
+        <v>1280</v>
+      </c>
+      <c r="G887" s="1" t="s">
+        <v>1284</v>
+      </c>
+      <c r="H887" s="1" t="s">
+        <v>1284</v>
+      </c>
+      <c r="I887" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="J887" s="1" t="s">
         <v>1279</v>
       </c>
-      <c r="F887" s="1" t="s">
-        <v>1281</v>
-      </c>
-      <c r="G887" s="1" t="s">
+      <c r="K887" s="9" t="s">
         <v>1285</v>
-      </c>
-      <c r="H887" s="1" t="s">
-        <v>1285</v>
-      </c>
-      <c r="I887" s="1" t="s">
-        <v>169</v>
-      </c>
-      <c r="J887" s="1" t="s">
-        <v>1280</v>
-      </c>
-      <c r="K887" s="9" t="s">
-        <v>1286</v>
       </c>
       <c r="M887" s="1" t="s">
         <v>954</v>
       </c>
       <c r="N887" s="1" t="s">
-        <v>1280</v>
+        <v>1279</v>
       </c>
       <c r="O887" s="1" t="s">
-        <v>1280</v>
+        <v>1279</v>
       </c>
       <c r="P887" s="1" t="s">
-        <v>1280</v>
+        <v>1279</v>
       </c>
       <c r="Q887" s="1" t="s">
-        <v>1280</v>
+        <v>1279</v>
       </c>
       <c r="S887" s="1" t="s">
-        <v>1280</v>
+        <v>1279</v>
       </c>
       <c r="X887" s="1" t="s">
-        <v>1280</v>
+        <v>1279</v>
       </c>
     </row>
     <row r="888" spans="1:24">
       <c r="A888" s="23" t="s">
-        <v>1270</v>
+        <v>1269</v>
       </c>
       <c r="D888" s="1" t="s">
+        <v>1278</v>
+      </c>
+      <c r="F888" s="1" t="s">
+        <v>1280</v>
+      </c>
+      <c r="G888" s="1" t="s">
+        <v>1284</v>
+      </c>
+      <c r="H888" s="1" t="s">
+        <v>1284</v>
+      </c>
+      <c r="I888" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="J888" s="1" t="s">
         <v>1279</v>
       </c>
-      <c r="F888" s="1" t="s">
-        <v>1281</v>
-      </c>
-      <c r="G888" s="1" t="s">
+      <c r="K888" s="9" t="s">
         <v>1285</v>
-      </c>
-      <c r="H888" s="1" t="s">
-        <v>1285</v>
-      </c>
-      <c r="I888" s="1" t="s">
-        <v>169</v>
-      </c>
-      <c r="J888" s="1" t="s">
-        <v>1280</v>
-      </c>
-      <c r="K888" s="9" t="s">
-        <v>1286</v>
       </c>
       <c r="M888" s="1" t="s">
         <v>954</v>
       </c>
       <c r="N888" s="1" t="s">
-        <v>1280</v>
+        <v>1279</v>
       </c>
       <c r="O888" s="1" t="s">
-        <v>1280</v>
+        <v>1279</v>
       </c>
       <c r="P888" s="1" t="s">
-        <v>1280</v>
+        <v>1279</v>
       </c>
       <c r="Q888" s="1" t="s">
-        <v>1280</v>
+        <v>1279</v>
       </c>
       <c r="S888" s="1" t="s">
-        <v>1280</v>
+        <v>1279</v>
       </c>
       <c r="X888" s="1" t="s">
-        <v>1280</v>
+        <v>1279</v>
       </c>
     </row>
     <row r="889" spans="1:24">
       <c r="A889" s="23" t="s">
-        <v>1271</v>
+        <v>1270</v>
       </c>
       <c r="D889" s="1" t="s">
+        <v>1278</v>
+      </c>
+      <c r="F889" s="1" t="s">
+        <v>1280</v>
+      </c>
+      <c r="G889" s="1" t="s">
+        <v>1284</v>
+      </c>
+      <c r="H889" s="1" t="s">
+        <v>1284</v>
+      </c>
+      <c r="I889" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="J889" s="1" t="s">
         <v>1279</v>
       </c>
-      <c r="F889" s="1" t="s">
-        <v>1281</v>
-      </c>
-      <c r="G889" s="1" t="s">
+      <c r="K889" s="9" t="s">
         <v>1285</v>
-      </c>
-      <c r="H889" s="1" t="s">
-        <v>1285</v>
-      </c>
-      <c r="I889" s="1" t="s">
-        <v>169</v>
-      </c>
-      <c r="J889" s="1" t="s">
-        <v>1280</v>
-      </c>
-      <c r="K889" s="9" t="s">
-        <v>1286</v>
       </c>
       <c r="M889" s="1" t="s">
         <v>954</v>
       </c>
       <c r="N889" s="1" t="s">
-        <v>1280</v>
+        <v>1279</v>
       </c>
       <c r="O889" s="1" t="s">
-        <v>1280</v>
+        <v>1279</v>
       </c>
       <c r="P889" s="1" t="s">
-        <v>1280</v>
+        <v>1279</v>
       </c>
       <c r="Q889" s="1" t="s">
-        <v>1280</v>
+        <v>1279</v>
       </c>
       <c r="S889" s="1" t="s">
-        <v>1280</v>
+        <v>1279</v>
       </c>
       <c r="X889" s="1" t="s">
-        <v>1280</v>
+        <v>1279</v>
       </c>
     </row>
     <row r="890" spans="1:24">
       <c r="A890" s="23" t="s">
-        <v>1272</v>
+        <v>1271</v>
       </c>
       <c r="D890" s="1" t="s">
+        <v>1278</v>
+      </c>
+      <c r="F890" s="1" t="s">
+        <v>1280</v>
+      </c>
+      <c r="G890" s="1" t="s">
+        <v>1284</v>
+      </c>
+      <c r="H890" s="1" t="s">
+        <v>1284</v>
+      </c>
+      <c r="I890" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="J890" s="1" t="s">
         <v>1279</v>
       </c>
-      <c r="F890" s="1" t="s">
-        <v>1281</v>
-      </c>
-      <c r="G890" s="1" t="s">
+      <c r="K890" s="9" t="s">
         <v>1285</v>
-      </c>
-      <c r="H890" s="1" t="s">
-        <v>1285</v>
-      </c>
-      <c r="I890" s="1" t="s">
-        <v>169</v>
-      </c>
-      <c r="J890" s="1" t="s">
-        <v>1280</v>
-      </c>
-      <c r="K890" s="9" t="s">
-        <v>1286</v>
       </c>
       <c r="M890" s="1" t="s">
         <v>954</v>
       </c>
       <c r="N890" s="1" t="s">
-        <v>1280</v>
+        <v>1279</v>
       </c>
       <c r="O890" s="1" t="s">
-        <v>1280</v>
+        <v>1279</v>
       </c>
       <c r="P890" s="1" t="s">
-        <v>1280</v>
+        <v>1279</v>
       </c>
       <c r="Q890" s="1" t="s">
-        <v>1280</v>
+        <v>1279</v>
       </c>
       <c r="S890" s="1" t="s">
-        <v>1280</v>
+        <v>1279</v>
       </c>
       <c r="X890" s="1" t="s">
-        <v>1280</v>
+        <v>1279</v>
       </c>
     </row>
     <row r="891" spans="1:24">
       <c r="A891" s="23" t="s">
-        <v>1273</v>
+        <v>1272</v>
       </c>
       <c r="D891" s="1" t="s">
+        <v>1278</v>
+      </c>
+      <c r="F891" s="1" t="s">
+        <v>1280</v>
+      </c>
+      <c r="G891" s="1" t="s">
+        <v>1284</v>
+      </c>
+      <c r="H891" s="1" t="s">
+        <v>1284</v>
+      </c>
+      <c r="I891" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="J891" s="1" t="s">
         <v>1279</v>
       </c>
-      <c r="F891" s="1" t="s">
-        <v>1281</v>
-      </c>
-      <c r="G891" s="1" t="s">
+      <c r="K891" s="9" t="s">
         <v>1285</v>
-      </c>
-      <c r="H891" s="1" t="s">
-        <v>1285</v>
-      </c>
-      <c r="I891" s="1" t="s">
-        <v>169</v>
-      </c>
-      <c r="J891" s="1" t="s">
-        <v>1280</v>
-      </c>
-      <c r="K891" s="9" t="s">
-        <v>1286</v>
       </c>
       <c r="M891" s="1" t="s">
         <v>954</v>
       </c>
       <c r="N891" s="1" t="s">
-        <v>1280</v>
+        <v>1279</v>
       </c>
       <c r="O891" s="1" t="s">
-        <v>1280</v>
+        <v>1279</v>
       </c>
       <c r="P891" s="1" t="s">
-        <v>1280</v>
+        <v>1279</v>
       </c>
       <c r="Q891" s="1" t="s">
-        <v>1280</v>
+        <v>1279</v>
       </c>
       <c r="S891" s="1" t="s">
-        <v>1280</v>
+        <v>1279</v>
       </c>
       <c r="X891" s="1" t="s">
-        <v>1280</v>
+        <v>1279</v>
       </c>
     </row>
     <row r="892" spans="1:24">
       <c r="A892" s="23" t="s">
-        <v>1274</v>
+        <v>1273</v>
       </c>
       <c r="D892" s="1" t="s">
+        <v>1278</v>
+      </c>
+      <c r="F892" s="1" t="s">
+        <v>1280</v>
+      </c>
+      <c r="G892" s="1" t="s">
+        <v>1284</v>
+      </c>
+      <c r="H892" s="1" t="s">
+        <v>1284</v>
+      </c>
+      <c r="I892" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="J892" s="1" t="s">
         <v>1279</v>
       </c>
-      <c r="F892" s="1" t="s">
-        <v>1281</v>
-      </c>
-      <c r="G892" s="1" t="s">
+      <c r="K892" s="9" t="s">
         <v>1285</v>
-      </c>
-      <c r="H892" s="1" t="s">
-        <v>1285</v>
-      </c>
-      <c r="I892" s="1" t="s">
-        <v>169</v>
-      </c>
-      <c r="J892" s="1" t="s">
-        <v>1280</v>
-      </c>
-      <c r="K892" s="9" t="s">
-        <v>1286</v>
       </c>
       <c r="M892" s="1" t="s">
         <v>954</v>
       </c>
       <c r="N892" s="1" t="s">
-        <v>1280</v>
+        <v>1279</v>
       </c>
       <c r="O892" s="1" t="s">
-        <v>1280</v>
+        <v>1279</v>
       </c>
       <c r="P892" s="1" t="s">
-        <v>1280</v>
+        <v>1279</v>
       </c>
       <c r="Q892" s="1" t="s">
-        <v>1280</v>
+        <v>1279</v>
       </c>
       <c r="S892" s="1" t="s">
-        <v>1280</v>
+        <v>1279</v>
       </c>
       <c r="X892" s="1" t="s">
-        <v>1280</v>
+        <v>1279</v>
       </c>
     </row>
   </sheetData>

</xml_diff>